<commit_message>
added pressure drop eqn for oil pipes (linearised darcy-weisbach)
</commit_message>
<xml_diff>
--- a/examples/data_example2.xlsx
+++ b/examples/data_example2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsven\code\OffshoreEnergySystem_OGESO\examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsven\code\OffshoreEnergySystem_OOGESO\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{987EDA10-3758-43D7-B124-EA70F8E9AF79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F2134FC-F5DB-4BE5-A56F-C94C3A9485CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11268" yWindow="2916" windowWidth="18252" windowHeight="12204" activeTab="3" xr2:uid="{67DC4D86-39E4-4DA3-B21D-C0F42277600B}"/>
+    <workbookView xWindow="7212" yWindow="2052" windowWidth="23040" windowHeight="12996" xr2:uid="{67DC4D86-39E4-4DA3-B21D-C0F42277600B}"/>
   </bookViews>
   <sheets>
     <sheet name="node" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="164">
   <si>
     <t>id</t>
   </si>
@@ -76,15 +76,9 @@
     <t>gas heater</t>
   </si>
   <si>
-    <t>heat pump</t>
-  </si>
-  <si>
     <t>heat demand</t>
   </si>
   <si>
-    <t>heat dump</t>
-  </si>
-  <si>
     <t>curve_wind</t>
   </si>
   <si>
@@ -118,9 +112,6 @@
     <t>gas EXPORT</t>
   </si>
   <si>
-    <t>el EXPORT</t>
-  </si>
-  <si>
     <t>compressor</t>
   </si>
   <si>
@@ -166,9 +157,6 @@
     <t>heat</t>
   </si>
   <si>
-    <t>heatpump</t>
-  </si>
-  <si>
     <t>length_km</t>
   </si>
   <si>
@@ -262,12 +250,6 @@
     <t>water</t>
   </si>
   <si>
-    <t>process_oil</t>
-  </si>
-  <si>
-    <t>process_water</t>
-  </si>
-  <si>
     <t>pump_oil</t>
   </si>
   <si>
@@ -292,9 +274,6 @@
     <t>powersupply</t>
   </si>
   <si>
-    <t>auxiliary</t>
-  </si>
-  <si>
     <t>oil EXPORT</t>
   </si>
   <si>
@@ -352,9 +331,6 @@
     <t>eta2</t>
   </si>
   <si>
-    <t>treatment_gas</t>
-  </si>
-  <si>
     <t>objective</t>
   </si>
   <si>
@@ -382,60 +358,24 @@
     <t>param_value</t>
   </si>
   <si>
-    <t>GT1</t>
-  </si>
-  <si>
-    <t>GT2</t>
-  </si>
-  <si>
-    <t>compr1</t>
-  </si>
-  <si>
-    <t>sep</t>
-  </si>
-  <si>
-    <t>aux</t>
-  </si>
-  <si>
-    <t>el load</t>
-  </si>
-  <si>
     <t>wind</t>
   </si>
   <si>
-    <t>diesel</t>
-  </si>
-  <si>
     <t>heat1</t>
   </si>
   <si>
     <t>water1</t>
   </si>
   <si>
-    <t>heat2</t>
-  </si>
-  <si>
     <t>ex_g</t>
   </si>
   <si>
     <t>ex_o</t>
   </si>
   <si>
-    <t>ex_e</t>
-  </si>
-  <si>
     <t>heat3</t>
   </si>
   <si>
-    <t>pump1</t>
-  </si>
-  <si>
-    <t>inj</t>
-  </si>
-  <si>
-    <t>water2</t>
-  </si>
-  <si>
     <t>kgCO2/MWh electricity</t>
   </si>
   <si>
@@ -445,9 +385,6 @@
     <t>MPa, wellhead pressure</t>
   </si>
   <si>
-    <t>compr2</t>
-  </si>
-  <si>
     <t>temp_in</t>
   </si>
   <si>
@@ -529,9 +466,6 @@
     <t>required electrical reserve</t>
   </si>
   <si>
-    <t>GT3</t>
-  </si>
-  <si>
     <t>gas turbine3</t>
   </si>
   <si>
@@ -551,6 +485,51 @@
   </si>
   <si>
     <t>pump efficiency - need possibly different model</t>
+  </si>
+  <si>
+    <t>Gen1</t>
+  </si>
+  <si>
+    <t>Gen2</t>
+  </si>
+  <si>
+    <t>Gen3</t>
+  </si>
+  <si>
+    <t>VSD_REC_01</t>
+  </si>
+  <si>
+    <t>PQ1</t>
+  </si>
+  <si>
+    <t>utility</t>
+  </si>
+  <si>
+    <t>general el load</t>
+  </si>
+  <si>
+    <t>Gen_EME_1</t>
+  </si>
+  <si>
+    <t>VSD_WIN</t>
+  </si>
+  <si>
+    <t>VSD_WST</t>
+  </si>
+  <si>
+    <t>VSD_OEX</t>
+  </si>
+  <si>
+    <t>VSD_SEP</t>
+  </si>
+  <si>
+    <t>water_injection</t>
+  </si>
+  <si>
+    <t>water_disp</t>
+  </si>
+  <si>
+    <t>height_m</t>
   </si>
 </sst>
 </file>
@@ -918,10 +897,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{052C0DB0-0590-4B7A-AC1E-E28475B8C302}">
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -948,39 +927,39 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B2">
         <v>-1</v>
@@ -992,7 +971,7 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H2">
         <v>2</v>
@@ -1003,7 +982,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>154</v>
       </c>
       <c r="B3">
         <v>-1</v>
@@ -1015,12 +994,12 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -1032,7 +1011,7 @@
         <v>-0.1</v>
       </c>
       <c r="E4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F4">
         <v>6</v>
@@ -1043,7 +1022,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>169</v>
+        <v>147</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -1055,7 +1034,7 @@
         <v>-0.1</v>
       </c>
       <c r="E5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F5">
         <v>6</v>
@@ -1066,7 +1045,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1078,7 +1057,7 @@
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F6">
         <v>6.5</v>
@@ -1095,7 +1074,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B7">
         <v>-1</v>
@@ -1107,18 +1086,18 @@
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J7">
         <v>0.3</v>
       </c>
       <c r="K7">
-        <v>0.3</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>76</v>
+        <v>32</v>
       </c>
       <c r="B8">
         <v>-1</v>
@@ -1130,18 +1109,18 @@
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
-      </c>
-      <c r="J8">
-        <v>0.3</v>
-      </c>
-      <c r="K8">
-        <v>3</v>
+        <v>15</v>
+      </c>
+      <c r="H8">
+        <v>2</v>
+      </c>
+      <c r="I8">
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>161</v>
       </c>
       <c r="B9">
         <v>-1</v>
@@ -1153,21 +1132,21 @@
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>17</v>
-      </c>
-      <c r="H9">
-        <v>2</v>
-      </c>
-      <c r="I9">
-        <v>10</v>
+        <v>15</v>
+      </c>
+      <c r="L9">
+        <v>0.7</v>
+      </c>
+      <c r="M9">
+        <v>0.7</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>104</v>
+        <v>51</v>
       </c>
       <c r="B10">
-        <v>-1</v>
+        <v>-1.2</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1176,64 +1155,18 @@
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H10">
-        <v>9.99</v>
+        <v>6.5</v>
       </c>
       <c r="I10">
-        <v>9.99</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>75</v>
-      </c>
-      <c r="B11">
-        <v>-1</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11" t="s">
-        <v>17</v>
-      </c>
-      <c r="L11">
-        <v>0.7</v>
-      </c>
-      <c r="M11">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>55</v>
-      </c>
-      <c r="B12">
-        <v>-1.2</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12" t="s">
-        <v>21</v>
-      </c>
-      <c r="H12">
-        <v>9.9700000000000006</v>
-      </c>
-      <c r="I12">
-        <v>9.9700000000000006</v>
-      </c>
-      <c r="J12">
+        <v>6.5</v>
+      </c>
+      <c r="J10">
         <v>3</v>
       </c>
-      <c r="K12">
+      <c r="K10">
         <v>3</v>
       </c>
     </row>
@@ -1245,10 +1178,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00A70904-C380-433D-9493-9658C938F213}">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1258,21 +1191,22 @@
     <col min="3" max="3" width="15.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.88671875" customWidth="1"/>
+    <col min="11" max="11" width="13.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>6</v>
@@ -1284,27 +1218,30 @@
         <v>8</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>45</v>
+        <v>163</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C2" t="s">
-        <v>84</v>
+        <v>154</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1322,15 +1259,15 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1348,15 +1285,15 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C4" t="s">
-        <v>74</v>
+        <v>161</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1374,15 +1311,15 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C5" t="s">
-        <v>104</v>
+        <v>32</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1400,15 +1337,15 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C6" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1426,15 +1363,15 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>147</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -1452,15 +1389,15 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="B8" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C8" t="s">
-        <v>76</v>
+        <v>154</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -1468,68 +1405,74 @@
       <c r="E8">
         <v>500</v>
       </c>
-      <c r="F8">
-        <v>1E-3</v>
-      </c>
-      <c r="G8">
-        <v>0.01</v>
-      </c>
-      <c r="H8">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>88</v>
       </c>
       <c r="B9" t="s">
-        <v>83</v>
+        <v>130</v>
       </c>
       <c r="C9" t="s">
-        <v>169</v>
+        <v>147</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="E9">
-        <v>500</v>
-      </c>
-      <c r="F9">
-        <v>1E-3</v>
-      </c>
-      <c r="G9">
-        <v>0.01</v>
+        <v>10000</v>
       </c>
       <c r="H9">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+        <v>0.1</v>
+      </c>
+      <c r="I9">
+        <v>200</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>88</v>
       </c>
       <c r="B10" t="s">
-        <v>83</v>
+        <v>147</v>
       </c>
       <c r="C10" t="s">
-        <v>84</v>
+        <v>25</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="E10">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+        <v>10000</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>200</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="B11" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="C11" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -1538,24 +1481,27 @@
         <v>10000</v>
       </c>
       <c r="H11">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="I11">
         <v>100</v>
       </c>
       <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
         <v>300</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>95</v>
+        <v>68</v>
       </c>
       <c r="B12" t="s">
-        <v>169</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>70</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -1564,24 +1510,27 @@
         <v>10000</v>
       </c>
       <c r="H12">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="I12">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
         <v>300</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>73</v>
+        <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>151</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>75</v>
+        <v>32</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -1590,24 +1539,27 @@
         <v>10000</v>
       </c>
       <c r="H13">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="I13">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
         <v>300</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>74</v>
+        <v>161</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -1622,18 +1574,21 @@
         <v>100</v>
       </c>
       <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
         <v>300</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C15" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -1642,24 +1597,27 @@
         <v>10000</v>
       </c>
       <c r="H15">
-        <v>0.01</v>
+        <v>5</v>
       </c>
       <c r="I15">
         <v>200</v>
       </c>
       <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
         <v>300</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>73</v>
+        <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -1674,18 +1632,21 @@
         <v>100</v>
       </c>
       <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
         <v>300</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B17" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C17" t="s">
-        <v>76</v>
+        <v>51</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -1694,163 +1655,33 @@
         <v>10000</v>
       </c>
       <c r="H17">
-        <v>0.01</v>
+        <v>5</v>
       </c>
       <c r="I17">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
         <v>300</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>77</v>
       </c>
       <c r="C18" t="s">
-        <v>104</v>
+        <v>25</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
       <c r="E18">
-        <v>10000</v>
-      </c>
-      <c r="H18">
-        <v>0.01</v>
-      </c>
-      <c r="I18">
-        <v>200</v>
-      </c>
-      <c r="J18">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" t="s">
-        <v>83</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19">
-        <v>10000</v>
-      </c>
-      <c r="H19">
-        <v>0.01</v>
-      </c>
-      <c r="I19">
-        <v>100</v>
-      </c>
-      <c r="J19">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>72</v>
-      </c>
-      <c r="B20" t="s">
-        <v>76</v>
-      </c>
-      <c r="C20" t="s">
-        <v>55</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20">
-        <v>10000</v>
-      </c>
-      <c r="H20">
-        <v>0.1</v>
-      </c>
-      <c r="I20">
-        <v>100</v>
-      </c>
-      <c r="J20">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21" t="s">
-        <v>104</v>
-      </c>
-      <c r="C21" t="s">
-        <v>55</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21">
-        <v>10000</v>
-      </c>
-      <c r="H21">
-        <v>0.1</v>
-      </c>
-      <c r="I21">
-        <v>200</v>
-      </c>
-      <c r="J21">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>41</v>
-      </c>
-      <c r="B22" t="s">
-        <v>83</v>
-      </c>
-      <c r="C22" t="s">
-        <v>28</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="E22">
         <v>1000</v>
-      </c>
-      <c r="H22">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>4</v>
-      </c>
-      <c r="B23" t="s">
-        <v>74</v>
-      </c>
-      <c r="C23" t="s">
-        <v>76</v>
-      </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="E23">
-        <v>500</v>
-      </c>
-      <c r="F23">
-        <v>1E-3</v>
-      </c>
-      <c r="G23">
-        <v>0.01</v>
-      </c>
-      <c r="H23">
-        <v>0.01</v>
       </c>
     </row>
   </sheetData>
@@ -1860,14 +1691,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB366907-93DA-4245-BEBF-19818450F8D2}">
-  <dimension ref="A1:J59"/>
+  <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.21875" bestFit="1" customWidth="1"/>
@@ -1883,28 +1715,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>10</v>
@@ -1912,19 +1744,19 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F2">
         <v>100</v>
@@ -1933,7 +1765,7 @@
         <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="I2">
         <v>0.5</v>
@@ -1941,19 +1773,19 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>114</v>
+        <v>149</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F3">
         <v>25</v>
@@ -1962,7 +1794,7 @@
         <v>10</v>
       </c>
       <c r="H3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I3">
         <v>2.35</v>
@@ -1970,7 +1802,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="I4">
         <v>0.53</v>
@@ -1978,7 +1810,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="I5">
         <v>0.05</v>
@@ -1986,18 +1818,18 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="I6">
         <v>0.5</v>
       </c>
       <c r="J6" t="s">
-        <v>158</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="I7">
         <v>1</v>
@@ -2005,41 +1837,41 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H8" t="s">
-        <v>153</v>
+        <v>132</v>
       </c>
       <c r="I8">
         <v>0</v>
       </c>
       <c r="J8" t="s">
-        <v>154</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H9" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
       <c r="I9">
         <v>200</v>
       </c>
       <c r="J9" t="s">
-        <v>159</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>115</v>
+        <v>150</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D10" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E10" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F10">
         <v>25</v>
@@ -2048,18 +1880,18 @@
         <v>10</v>
       </c>
       <c r="H10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I10">
-        <v>2.36</v>
+        <v>2.3519999999999999</v>
       </c>
       <c r="J10" t="s">
-        <v>156</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="I11">
         <v>0.53</v>
@@ -2067,7 +1899,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H12" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="I12">
         <v>0.05</v>
@@ -2075,7 +1907,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H13" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="I13">
         <v>0.5</v>
@@ -2083,7 +1915,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H14" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="I14">
         <v>1</v>
@@ -2091,41 +1923,41 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H15" t="s">
-        <v>153</v>
+        <v>132</v>
       </c>
       <c r="I15">
         <v>0</v>
       </c>
       <c r="J15" t="s">
-        <v>154</v>
+        <v>133</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H16" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
       <c r="I16">
         <v>200</v>
       </c>
       <c r="J16" t="s">
-        <v>159</v>
+        <v>138</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D17" t="s">
-        <v>164</v>
+        <v>142</v>
       </c>
       <c r="E17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F17">
         <v>25</v>
@@ -2134,18 +1966,18 @@
         <v>10</v>
       </c>
       <c r="H17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I17">
-        <v>2.37</v>
+        <v>2.3540000000000001</v>
       </c>
       <c r="J17" t="s">
-        <v>156</v>
+        <v>135</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H18" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="I18">
         <v>0.53</v>
@@ -2153,7 +1985,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H19" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="I19">
         <v>0.05</v>
@@ -2161,7 +1993,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H20" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="I20">
         <v>0.5</v>
@@ -2169,7 +2001,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H21" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="I21">
         <v>1</v>
@@ -2177,41 +2009,41 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H22" t="s">
-        <v>153</v>
+        <v>132</v>
       </c>
       <c r="I22">
         <v>0</v>
       </c>
       <c r="J22" t="s">
-        <v>154</v>
+        <v>133</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H23" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
       <c r="I23">
         <v>200</v>
       </c>
       <c r="J23" t="s">
-        <v>159</v>
+        <v>138</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>116</v>
+        <v>156</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C24" t="s">
-        <v>35</v>
+        <v>77</v>
       </c>
       <c r="D24" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E24" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="F24">
         <v>1000</v>
@@ -2220,741 +2052,615 @@
         <v>0</v>
       </c>
       <c r="H24" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="I24">
+        <f>270/0.1</f>
+        <v>2700</v>
+      </c>
+      <c r="J24" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>152</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" t="s">
+        <v>24</v>
+      </c>
+      <c r="E25" t="s">
+        <v>29</v>
+      </c>
+      <c r="F25">
+        <v>1000</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25" t="s">
+        <v>33</v>
+      </c>
+      <c r="I25">
         <v>0.4</v>
       </c>
-      <c r="J24" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H25" t="s">
-        <v>136</v>
-      </c>
-      <c r="I25">
+      <c r="J25" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H26" t="s">
+        <v>115</v>
+      </c>
+      <c r="I26">
         <v>300</v>
       </c>
-      <c r="J25" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H26" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="I26">
+      <c r="J26" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H27" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="I27">
         <v>20</v>
       </c>
-      <c r="J26" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>135</v>
-      </c>
-      <c r="B27">
+      <c r="J27" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>160</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28" t="s">
+        <v>25</v>
+      </c>
+      <c r="E28" t="s">
+        <v>25</v>
+      </c>
+      <c r="F28">
+        <v>1000</v>
+      </c>
+      <c r="G28">
         <v>0</v>
       </c>
-      <c r="C27" t="s">
-        <v>35</v>
-      </c>
-      <c r="D27" t="s">
-        <v>27</v>
-      </c>
-      <c r="E27" t="s">
-        <v>35</v>
-      </c>
-      <c r="F27">
-        <v>1000</v>
-      </c>
-      <c r="G27">
-        <v>0</v>
-      </c>
-      <c r="H27" t="s">
-        <v>36</v>
-      </c>
-      <c r="I27">
-        <v>0.2</v>
-      </c>
-      <c r="J27" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H28" t="s">
-        <v>136</v>
-      </c>
-      <c r="I28">
-        <v>300</v>
-      </c>
-      <c r="J28" t="s">
-        <v>137</v>
+      <c r="H28" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I28" s="2">
+        <v>0.1</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H29" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="I29">
-        <v>20</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>140</v>
+        <v>96</v>
+      </c>
+      <c r="I29" s="2">
+        <v>0.1</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>117</v>
+        <v>153</v>
       </c>
       <c r="B30">
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>28</v>
+        <v>154</v>
       </c>
       <c r="D30" t="s">
-        <v>28</v>
+        <v>155</v>
       </c>
       <c r="E30" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F30">
-        <v>1000</v>
+        <v>5</v>
       </c>
       <c r="G30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>106</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31" t="s">
+        <v>77</v>
+      </c>
+      <c r="D31" t="s">
+        <v>21</v>
+      </c>
+      <c r="E31" t="s">
+        <v>49</v>
+      </c>
+      <c r="F31">
+        <v>20</v>
+      </c>
+      <c r="G31">
         <v>0</v>
       </c>
-      <c r="H30" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I30" s="2">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H31" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="I31" s="2">
-        <v>0.1</v>
+      <c r="H31" t="s">
+        <v>127</v>
+      </c>
+      <c r="I31" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>118</v>
-      </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
-      <c r="C32" t="s">
-        <v>84</v>
-      </c>
-      <c r="D32" t="s">
-        <v>119</v>
-      </c>
-      <c r="E32" t="s">
-        <v>33</v>
-      </c>
-      <c r="F32">
-        <v>5</v>
-      </c>
-      <c r="G32">
-        <v>3</v>
+      <c r="H32" t="s">
+        <v>50</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="J32" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>83</v>
+        <v>154</v>
       </c>
       <c r="D33" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" t="s">
+        <v>36</v>
+      </c>
+      <c r="F33">
+        <v>5</v>
+      </c>
+      <c r="G33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>109</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D34" t="s">
         <v>23</v>
       </c>
-      <c r="E33" t="s">
-        <v>53</v>
-      </c>
-      <c r="F33">
-        <v>20</v>
-      </c>
-      <c r="G33">
+      <c r="E34" t="s">
+        <v>79</v>
+      </c>
+      <c r="F34">
+        <v>1000</v>
+      </c>
+      <c r="G34">
         <v>0</v>
-      </c>
-      <c r="H33" t="s">
-        <v>148</v>
-      </c>
-      <c r="I33" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H34" t="s">
-        <v>54</v>
-      </c>
-      <c r="I34">
-        <v>0</v>
-      </c>
-      <c r="J34" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>42</v>
+        <v>110</v>
       </c>
       <c r="B35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>84</v>
+        <v>51</v>
       </c>
       <c r="D35" t="s">
-        <v>12</v>
+        <v>78</v>
       </c>
       <c r="E35" t="s">
-        <v>42</v>
+        <v>80</v>
       </c>
       <c r="F35">
-        <v>5</v>
+        <v>1000</v>
       </c>
       <c r="G35">
         <v>0</v>
       </c>
-      <c r="H35" t="s">
-        <v>36</v>
-      </c>
-      <c r="I35">
-        <v>3</v>
-      </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="B36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C36" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D36" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E36" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F36">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G36">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>124</v>
+        <v>61</v>
       </c>
       <c r="B37">
         <v>0</v>
       </c>
       <c r="C37" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D37" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="E37" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="F37">
-        <v>1000</v>
+        <v>4</v>
       </c>
       <c r="G37">
         <v>0</v>
       </c>
+      <c r="H37" t="s">
+        <v>33</v>
+      </c>
+      <c r="I37">
+        <v>0.9</v>
+      </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+      <c r="H38" t="s">
+        <v>63</v>
+      </c>
+      <c r="I38">
+        <v>2</v>
+      </c>
+      <c r="J38" t="s">
         <v>125</v>
-      </c>
-      <c r="B38">
-        <v>1</v>
-      </c>
-      <c r="C38" t="s">
-        <v>55</v>
-      </c>
-      <c r="D38" t="s">
-        <v>25</v>
-      </c>
-      <c r="E38" t="s">
-        <v>86</v>
-      </c>
-      <c r="F38">
-        <v>1000</v>
-      </c>
-      <c r="G38">
-        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>126</v>
+        <v>64</v>
       </c>
       <c r="B39">
         <v>1</v>
       </c>
       <c r="C39" t="s">
-        <v>55</v>
+        <v>130</v>
       </c>
       <c r="D39" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="E39" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="F39">
-        <v>1000</v>
+        <v>15</v>
       </c>
       <c r="G39">
         <v>0</v>
       </c>
+      <c r="H39" t="s">
+        <v>42</v>
+      </c>
+      <c r="I39">
+        <v>6</v>
+      </c>
+      <c r="J39" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+      <c r="H40" t="s">
         <v>127</v>
       </c>
-      <c r="B40">
-        <v>0</v>
-      </c>
-      <c r="C40" t="s">
-        <v>55</v>
-      </c>
-      <c r="D40" t="s">
-        <v>26</v>
-      </c>
-      <c r="E40" t="s">
-        <v>33</v>
-      </c>
-      <c r="F40">
-        <v>1000</v>
-      </c>
-      <c r="G40">
-        <v>0</v>
+      <c r="I40" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>121</v>
+        <v>65</v>
       </c>
       <c r="B41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>83</v>
+        <v>130</v>
       </c>
       <c r="D41" t="s">
-        <v>24</v>
+        <v>65</v>
       </c>
       <c r="E41" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="F41">
-        <v>1000</v>
+        <v>35</v>
       </c>
       <c r="G41">
         <v>0</v>
       </c>
       <c r="H41" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="I41">
-        <f>270/0.1</f>
-        <v>2700</v>
+        <v>6</v>
       </c>
       <c r="J41" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>128</v>
-      </c>
-      <c r="B42">
-        <v>0</v>
-      </c>
-      <c r="C42" t="s">
-        <v>83</v>
-      </c>
-      <c r="D42" t="s">
-        <v>13</v>
-      </c>
-      <c r="E42" t="s">
-        <v>39</v>
-      </c>
-      <c r="F42">
-        <v>4</v>
-      </c>
-      <c r="G42">
-        <v>2</v>
+      <c r="H42" t="s">
+        <v>127</v>
+      </c>
+      <c r="I42" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C43" t="s">
-        <v>83</v>
+        <v>130</v>
       </c>
       <c r="D43" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E43" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F43">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="G43">
         <v>0</v>
       </c>
       <c r="H43" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="I43">
-        <v>0.9</v>
+        <v>6</v>
+      </c>
+      <c r="J43" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H44" t="s">
-        <v>67</v>
-      </c>
-      <c r="I44">
-        <v>2</v>
-      </c>
-      <c r="J44" t="s">
-        <v>146</v>
+        <v>127</v>
+      </c>
+      <c r="I44" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>68</v>
+        <v>159</v>
       </c>
       <c r="B45">
         <v>1</v>
       </c>
       <c r="C45" t="s">
-        <v>151</v>
+        <v>70</v>
       </c>
       <c r="D45" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
       <c r="E45" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F45">
-        <v>15</v>
+        <v>1000</v>
       </c>
       <c r="G45">
         <v>0</v>
       </c>
       <c r="H45" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="I45">
-        <v>6</v>
+        <v>0.8</v>
       </c>
       <c r="J45" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H46" t="s">
+      <c r="A46" t="s">
+        <v>158</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46" t="s">
+        <v>147</v>
+      </c>
+      <c r="D46" t="s">
+        <v>145</v>
+      </c>
+      <c r="E46" t="s">
+        <v>146</v>
+      </c>
+      <c r="F46">
+        <v>1000</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I46" s="2">
+        <v>3</v>
+      </c>
+      <c r="J46" s="2" t="s">
         <v>148</v>
-      </c>
-      <c r="I46" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>69</v>
+        <v>157</v>
       </c>
       <c r="B47">
         <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="D47" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="E47" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F47">
-        <v>35</v>
+        <v>1.3</v>
       </c>
       <c r="G47">
-        <v>0</v>
+        <v>1.3</v>
       </c>
       <c r="H47" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="I47">
-        <v>6</v>
+        <v>0.8</v>
       </c>
       <c r="J47" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H48" t="s">
-        <v>148</v>
-      </c>
-      <c r="I48" t="s">
-        <v>52</v>
+        <v>121</v>
+      </c>
+      <c r="I48">
+        <v>6</v>
+      </c>
+      <c r="J48" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>70</v>
-      </c>
-      <c r="B49">
-        <v>0</v>
-      </c>
-      <c r="C49" t="s">
-        <v>151</v>
-      </c>
-      <c r="D49" t="s">
-        <v>70</v>
-      </c>
-      <c r="E49" t="s">
-        <v>71</v>
-      </c>
-      <c r="F49">
-        <v>20</v>
-      </c>
-      <c r="G49">
-        <v>0</v>
-      </c>
       <c r="H49" t="s">
-        <v>46</v>
+        <v>124</v>
       </c>
       <c r="I49">
-        <v>6</v>
+        <v>1.3</v>
       </c>
       <c r="J49" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H50" t="s">
-        <v>148</v>
-      </c>
-      <c r="I50" t="s">
-        <v>52</v>
+        <v>63</v>
+      </c>
+      <c r="I50">
+        <v>1.3</v>
+      </c>
+      <c r="J50" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>131</v>
-      </c>
-      <c r="B51">
-        <v>0</v>
-      </c>
-      <c r="C51" t="s">
-        <v>75</v>
-      </c>
-      <c r="D51" t="s">
-        <v>88</v>
-      </c>
-      <c r="E51" t="s">
-        <v>89</v>
-      </c>
-      <c r="F51">
-        <v>1000</v>
-      </c>
-      <c r="G51">
-        <v>0</v>
+      <c r="H51" t="s">
+        <v>143</v>
+      </c>
+      <c r="I51">
+        <v>1</v>
+      </c>
+      <c r="J51" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
       <c r="B52">
         <v>1</v>
       </c>
       <c r="C52" t="s">
-        <v>76</v>
+        <v>130</v>
       </c>
       <c r="D52" t="s">
-        <v>92</v>
+        <v>131</v>
       </c>
       <c r="E52" t="s">
-        <v>76</v>
+        <v>103</v>
       </c>
       <c r="F52">
-        <v>1000</v>
+        <v>5</v>
       </c>
       <c r="G52">
         <v>0</v>
       </c>
       <c r="H52" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="I52">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="J52" t="s">
-        <v>141</v>
+        <v>113</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C53" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="D53" t="s">
-        <v>167</v>
+        <v>81</v>
       </c>
       <c r="E53" t="s">
-        <v>168</v>
+        <v>82</v>
       </c>
       <c r="F53">
         <v>1000</v>
       </c>
       <c r="G53">
         <v>0</v>
-      </c>
-      <c r="H53" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I53" s="2">
-        <v>3</v>
-      </c>
-      <c r="J53" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>130</v>
-      </c>
-      <c r="B54">
-        <v>1</v>
-      </c>
-      <c r="C54" t="s">
-        <v>75</v>
-      </c>
-      <c r="D54" t="s">
-        <v>93</v>
-      </c>
-      <c r="E54" t="s">
-        <v>94</v>
-      </c>
-      <c r="F54">
-        <v>1.3</v>
-      </c>
-      <c r="G54">
-        <v>1.3</v>
-      </c>
-      <c r="H54" t="s">
-        <v>36</v>
-      </c>
-      <c r="I54">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H55" t="s">
-        <v>142</v>
-      </c>
-      <c r="I55">
-        <v>6</v>
-      </c>
-      <c r="J55" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H56" t="s">
-        <v>145</v>
-      </c>
-      <c r="I56">
-        <v>1.3</v>
-      </c>
-      <c r="J56" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H57" t="s">
-        <v>67</v>
-      </c>
-      <c r="I57">
-        <v>1.3</v>
-      </c>
-      <c r="J57" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H58" t="s">
-        <v>165</v>
-      </c>
-      <c r="I58">
-        <v>1</v>
-      </c>
-      <c r="J58" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>123</v>
-      </c>
-      <c r="B59">
-        <v>1</v>
-      </c>
-      <c r="C59" t="s">
-        <v>151</v>
-      </c>
-      <c r="D59" t="s">
-        <v>152</v>
-      </c>
-      <c r="E59" t="s">
-        <v>111</v>
-      </c>
-      <c r="F59">
-        <v>5</v>
-      </c>
-      <c r="G59">
-        <v>0</v>
-      </c>
-      <c r="H59" t="s">
-        <v>46</v>
-      </c>
-      <c r="I59">
-        <v>0.7</v>
-      </c>
-      <c r="J59" t="s">
-        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -2967,7 +2673,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98F6EB10-AB47-4D11-878D-7EA50574CBA2}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
@@ -2980,10 +2686,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C1" t="s">
         <v>10</v>
@@ -2991,145 +2697,145 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B2">
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B3">
         <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>155</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B4">
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>150</v>
+        <v>129</v>
       </c>
       <c r="B5">
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>149</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="B6">
         <v>0.04</v>
       </c>
       <c r="C6" t="s">
-        <v>157</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B7" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C7" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B8">
         <v>0.05</v>
       </c>
       <c r="C8" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B9">
         <v>-1</v>
       </c>
       <c r="C9" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="B10">
         <v>-1</v>
       </c>
       <c r="C10" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="B11" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C11" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="B12" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="C12" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>161</v>
+        <v>140</v>
       </c>
       <c r="B13">
         <v>0.5</v>
       </c>
       <c r="C13" t="s">
-        <v>162</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="B14" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C14" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -3141,7 +2847,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3E6B22F-D4D7-489D-AE2A-F030E504A301}">
   <dimension ref="A1:C290"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -3149,13 +2855,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -6352,13 +6058,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
reorganised optimisation problem code (removed superfluous "devicePower" variable)
</commit_message>
<xml_diff>
--- a/examples/data_example2.xlsx
+++ b/examples/data_example2.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsven\code\OffshoreEnergySystem_OOGESO\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F2134FC-F5DB-4BE5-A56F-C94C3A9485CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE6057C8-59D7-4700-97CF-103A9B030E01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7212" yWindow="2052" windowWidth="23040" windowHeight="12996" xr2:uid="{67DC4D86-39E4-4DA3-B21D-C0F42277600B}"/>
+    <workbookView xWindow="5064" yWindow="3516" windowWidth="23040" windowHeight="12996" activeTab="3" xr2:uid="{67DC4D86-39E4-4DA3-B21D-C0F42277600B}"/>
   </bookViews>
   <sheets>
     <sheet name="node" sheetId="1" r:id="rId1"/>
     <sheet name="edge" sheetId="2" r:id="rId2"/>
     <sheet name="device" sheetId="7" r:id="rId3"/>
-    <sheet name="parameters" sheetId="4" r:id="rId4"/>
-    <sheet name="profiles" sheetId="5" r:id="rId5"/>
-    <sheet name="profiles_forecast" sheetId="6" r:id="rId6"/>
+    <sheet name="carriers" sheetId="8" r:id="rId4"/>
+    <sheet name="parameters" sheetId="4" r:id="rId5"/>
+    <sheet name="profiles" sheetId="5" r:id="rId6"/>
+    <sheet name="profiles_forecast" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="207">
   <si>
     <t>id</t>
   </si>
@@ -58,12 +59,6 @@
     <t>gas</t>
   </si>
   <si>
-    <t>capacity</t>
-  </si>
-  <si>
-    <t>reistance</t>
-  </si>
-  <si>
     <t>reactance</t>
   </si>
   <si>
@@ -82,9 +77,6 @@
     <t>curve_wind</t>
   </si>
   <si>
-    <t>coord_z</t>
-  </si>
-  <si>
     <t>platform</t>
   </si>
   <si>
@@ -169,12 +161,6 @@
     <t>naturalpressure</t>
   </si>
   <si>
-    <t>parameter</t>
-  </si>
-  <si>
-    <t>value</t>
-  </si>
-  <si>
     <t>planning_horizon</t>
   </si>
   <si>
@@ -253,24 +239,6 @@
     <t>pump_oil</t>
   </si>
   <si>
-    <t>pressure.oil.in</t>
-  </si>
-  <si>
-    <t>pressure.oil.out</t>
-  </si>
-  <si>
-    <t>pressure.water.in</t>
-  </si>
-  <si>
-    <t>pressure.water.out</t>
-  </si>
-  <si>
-    <t>pressure.gas.in</t>
-  </si>
-  <si>
-    <t>pressure.gas.out</t>
-  </si>
-  <si>
     <t>powersupply</t>
   </si>
   <si>
@@ -307,12 +275,6 @@
     <t>wellstream</t>
   </si>
   <si>
-    <t>pressure.wellstream.out</t>
-  </si>
-  <si>
-    <t>pressure.wellstream.in</t>
-  </si>
-  <si>
     <t>emissionRateMax</t>
   </si>
   <si>
@@ -412,9 +374,6 @@
     <t>Sm3/s (must be between Pmin and Pmax)</t>
   </si>
   <si>
-    <t>Pavg</t>
-  </si>
-  <si>
     <t>MWh (1/2 hour at full power)</t>
   </si>
   <si>
@@ -530,6 +489,177 @@
   </si>
   <si>
     <t>height_m</t>
+  </si>
+  <si>
+    <t>Qmax</t>
+  </si>
+  <si>
+    <t>Sm3/s</t>
+  </si>
+  <si>
+    <t>Qmin</t>
+  </si>
+  <si>
+    <t>rho_density</t>
+  </si>
+  <si>
+    <t>viscosity</t>
+  </si>
+  <si>
+    <t>export_price</t>
+  </si>
+  <si>
+    <t>darcy_friction</t>
+  </si>
+  <si>
+    <t>energy_value</t>
+  </si>
+  <si>
+    <t>CO2content</t>
+  </si>
+  <si>
+    <t>Tb_basetemp_K</t>
+  </si>
+  <si>
+    <t>Pb_basepressure_MPa</t>
+  </si>
+  <si>
+    <t>G_gravity</t>
+  </si>
+  <si>
+    <t>Z_compressibility</t>
+  </si>
+  <si>
+    <t>k_heat_capacity_ratio</t>
+  </si>
+  <si>
+    <t>R_individual_gas_constant</t>
+  </si>
+  <si>
+    <t>kg/m3</t>
+  </si>
+  <si>
+    <t>kg/(m s)</t>
+  </si>
+  <si>
+    <t>$/Sm3</t>
+  </si>
+  <si>
+    <t>MJ/Sm3</t>
+  </si>
+  <si>
+    <t>atmospheric pressure</t>
+  </si>
+  <si>
+    <t>15 deg C</t>
+  </si>
+  <si>
+    <t>J/(kg K)</t>
+  </si>
+  <si>
+    <t>no parameters</t>
+  </si>
+  <si>
+    <t>resistance</t>
+  </si>
+  <si>
+    <t>pressure.from</t>
+  </si>
+  <si>
+    <t>pressure.to</t>
+  </si>
+  <si>
+    <t>e1</t>
+  </si>
+  <si>
+    <t>e2</t>
+  </si>
+  <si>
+    <t>e3</t>
+  </si>
+  <si>
+    <t>e4</t>
+  </si>
+  <si>
+    <t>e5</t>
+  </si>
+  <si>
+    <t>e6</t>
+  </si>
+  <si>
+    <t>h1</t>
+  </si>
+  <si>
+    <t>h2</t>
+  </si>
+  <si>
+    <t>w1</t>
+  </si>
+  <si>
+    <t>w2</t>
+  </si>
+  <si>
+    <t>o1</t>
+  </si>
+  <si>
+    <t>o2</t>
+  </si>
+  <si>
+    <t>g1</t>
+  </si>
+  <si>
+    <t>g2</t>
+  </si>
+  <si>
+    <t>g3</t>
+  </si>
+  <si>
+    <t>c1</t>
+  </si>
+  <si>
+    <t>c2</t>
+  </si>
+  <si>
+    <t>Qavg</t>
+  </si>
+  <si>
+    <t>Vmax</t>
+  </si>
+  <si>
+    <t>maxdeviation_pressure.gas.in</t>
+  </si>
+  <si>
+    <t>maxdeviation_pressure.oil.in</t>
+  </si>
+  <si>
+    <t>comment2</t>
+  </si>
+  <si>
+    <t>no slack</t>
+  </si>
+  <si>
+    <t>composition.oil</t>
+  </si>
+  <si>
+    <t>composition.gas</t>
+  </si>
+  <si>
+    <t>composition.water</t>
+  </si>
+  <si>
+    <t>Sm3 fraction</t>
+  </si>
+  <si>
+    <t>desc</t>
+  </si>
+  <si>
+    <t>kg/m3, computed from composition and densities of gas/oil/water</t>
+  </si>
+  <si>
+    <t>kg/(m s) - assuming quite light crude (lot of gas)</t>
+  </si>
+  <si>
+    <t>kg/Sm3 - SSB 2016 report</t>
   </si>
 </sst>
 </file>
@@ -579,10 +709,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -897,277 +1028,191 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{052C0DB0-0590-4B7A-AC1E-E28475B8C302}">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="14.33203125" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B2">
+        <v>66</v>
+      </c>
+      <c r="F2">
         <v>-1</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F3">
+        <v>-1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>116</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
         <v>0</v>
       </c>
-      <c r="E2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2">
+      <c r="H4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>133</v>
+      </c>
+      <c r="F5">
         <v>2</v>
       </c>
-      <c r="I2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>154</v>
-      </c>
-      <c r="B3">
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F7">
         <v>-1</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>130</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>-0.1</v>
-      </c>
-      <c r="E4" t="s">
-        <v>52</v>
-      </c>
-      <c r="F4">
-        <v>6</v>
-      </c>
-      <c r="G4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8">
+        <v>-1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>147</v>
       </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>-0.1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F5">
-        <v>6</v>
-      </c>
-      <c r="G5">
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6">
-        <v>6.5</v>
-      </c>
-      <c r="I6">
-        <v>2</v>
-      </c>
-      <c r="K6">
-        <v>0.3</v>
-      </c>
-      <c r="M6">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>70</v>
-      </c>
-      <c r="B7">
+      <c r="F9">
         <v>-1</v>
       </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7" t="s">
-        <v>15</v>
-      </c>
-      <c r="J7">
-        <v>0.3</v>
-      </c>
-      <c r="K7">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8">
-        <v>-1</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8">
-        <v>2</v>
-      </c>
-      <c r="I8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>161</v>
-      </c>
-      <c r="B9">
-        <v>-1</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9" t="s">
-        <v>15</v>
-      </c>
-      <c r="L9">
-        <v>0.7</v>
-      </c>
-      <c r="M9">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10">
-        <v>-1.2</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
+        <v>46</v>
+      </c>
+      <c r="C10" t="s">
+        <v>195</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>19</v>
-      </c>
-      <c r="H10">
-        <v>6.5</v>
-      </c>
-      <c r="I10">
-        <v>6.5</v>
-      </c>
-      <c r="J10">
-        <v>3</v>
-      </c>
-      <c r="K10">
-        <v>3</v>
+        <v>198</v>
+      </c>
+      <c r="F10">
+        <v>-1.2</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>196</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -1178,510 +1223,754 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00A70904-C380-433D-9493-9658C938F213}">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:H52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.88671875" customWidth="1"/>
-    <col min="11" max="11" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>0.01</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G3" t="s">
+        <v>173</v>
+      </c>
+      <c r="H3">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G4" t="s">
         <v>6</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C2" t="s">
-        <v>154</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>500</v>
-      </c>
-      <c r="F2">
-        <v>1E-3</v>
-      </c>
-      <c r="G2">
-        <v>0.01</v>
-      </c>
-      <c r="H2">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>500</v>
-      </c>
-      <c r="F3">
-        <v>1E-3</v>
-      </c>
-      <c r="G3">
-        <v>0.01</v>
-      </c>
-      <c r="H3">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C4" t="s">
-        <v>161</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>500</v>
-      </c>
-      <c r="F4">
-        <v>1E-3</v>
-      </c>
-      <c r="G4">
-        <v>0.01</v>
       </c>
       <c r="H4">
         <v>0.01</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>77</v>
-      </c>
       <c r="C5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
+        <v>66</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
       </c>
       <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>0.01</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5">
         <v>500</v>
       </c>
-      <c r="F5">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G6" t="s">
+        <v>173</v>
+      </c>
+      <c r="H6">
         <v>1E-3</v>
       </c>
-      <c r="G5">
-        <v>0.01</v>
-      </c>
-      <c r="H5">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>77</v>
-      </c>
-      <c r="C6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>500</v>
-      </c>
-      <c r="F6">
-        <v>1E-3</v>
-      </c>
-      <c r="G6">
-        <v>0.01</v>
-      </c>
-      <c r="H6">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>77</v>
-      </c>
-      <c r="C7" t="s">
-        <v>147</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>500</v>
-      </c>
-      <c r="F7">
-        <v>1E-3</v>
-      </c>
-      <c r="G7">
-        <v>0.01</v>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G7" t="s">
+        <v>6</v>
       </c>
       <c r="H7">
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>178</v>
       </c>
       <c r="B8" t="s">
-        <v>77</v>
+        <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>154</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
+        <v>66</v>
+      </c>
+      <c r="D8" t="s">
+        <v>147</v>
       </c>
       <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>0.01</v>
+      </c>
+      <c r="G8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8">
         <v>500</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>88</v>
-      </c>
-      <c r="B9" t="s">
-        <v>130</v>
-      </c>
-      <c r="C9" t="s">
-        <v>147</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>10000</v>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G9" t="s">
+        <v>173</v>
       </c>
       <c r="H9">
-        <v>0.1</v>
-      </c>
-      <c r="I9">
-        <v>200</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="K9">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>88</v>
-      </c>
-      <c r="B10" t="s">
-        <v>147</v>
-      </c>
-      <c r="C10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <v>10000</v>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G10" t="s">
+        <v>6</v>
       </c>
       <c r="H10">
-        <v>1</v>
-      </c>
-      <c r="I10">
-        <v>200</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>69</v>
+        <v>179</v>
       </c>
       <c r="B11" t="s">
-        <v>130</v>
+        <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>161</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
+        <v>66</v>
+      </c>
+      <c r="D11" t="s">
+        <v>29</v>
       </c>
       <c r="E11">
-        <v>10000</v>
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>0.01</v>
+      </c>
+      <c r="G11" t="s">
+        <v>13</v>
       </c>
       <c r="H11">
-        <v>1</v>
-      </c>
-      <c r="I11">
-        <v>100</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>68</v>
-      </c>
-      <c r="B12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" t="s">
-        <v>70</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12">
-        <v>10000</v>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G12" t="s">
+        <v>173</v>
       </c>
       <c r="H12">
-        <v>0.01</v>
-      </c>
-      <c r="I12">
-        <v>200</v>
-      </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
-      <c r="K12">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13">
-        <v>10000</v>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G13" t="s">
+        <v>6</v>
       </c>
       <c r="H13">
         <v>0.01</v>
       </c>
-      <c r="I13">
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>180</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>0.01</v>
+      </c>
+      <c r="G14" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14">
         <v>500</v>
       </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
-      <c r="K13">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>69</v>
-      </c>
-      <c r="B14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" t="s">
-        <v>161</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14">
-        <v>10000</v>
-      </c>
-      <c r="H14">
-        <v>0.01</v>
-      </c>
-      <c r="I14">
-        <v>100</v>
-      </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
-      <c r="K14">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15">
-        <v>10000</v>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G15" t="s">
+        <v>173</v>
       </c>
       <c r="H15">
-        <v>5</v>
-      </c>
-      <c r="I15">
-        <v>200</v>
-      </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
-      <c r="K15">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" t="s">
-        <v>77</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16">
-        <v>10000</v>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G16" t="s">
+        <v>6</v>
       </c>
       <c r="H16">
         <v>0.01</v>
       </c>
-      <c r="I16">
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>181</v>
+      </c>
+      <c r="B17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>0.01</v>
+      </c>
+      <c r="G17" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G18" t="s">
+        <v>173</v>
+      </c>
+      <c r="H18">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G19" t="s">
+        <v>6</v>
+      </c>
+      <c r="H19">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>182</v>
+      </c>
+      <c r="B20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" t="s">
+        <v>140</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="G20" t="s">
+        <v>13</v>
+      </c>
+      <c r="H20">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>183</v>
+      </c>
+      <c r="B21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" t="s">
+        <v>66</v>
+      </c>
+      <c r="D21" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="G21" t="s">
+        <v>13</v>
+      </c>
+      <c r="H21">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>191</v>
+      </c>
+      <c r="B22" t="s">
+        <v>77</v>
+      </c>
+      <c r="C22" t="s">
+        <v>116</v>
+      </c>
+      <c r="D22" t="s">
+        <v>133</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>0.1</v>
+      </c>
+      <c r="G22" t="s">
+        <v>37</v>
+      </c>
+      <c r="H22">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G23" t="s">
+        <v>174</v>
+      </c>
+      <c r="H23">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G24" t="s">
+        <v>175</v>
+      </c>
+      <c r="H24">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>192</v>
+      </c>
+      <c r="B25" t="s">
+        <v>77</v>
+      </c>
+      <c r="C25" t="s">
+        <v>133</v>
+      </c>
+      <c r="D25" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25" t="s">
+        <v>37</v>
+      </c>
+      <c r="H25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G26" t="s">
+        <v>174</v>
+      </c>
+      <c r="H26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G27" t="s">
+        <v>175</v>
+      </c>
+      <c r="H27">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G28" t="s">
+        <v>149</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>186</v>
+      </c>
+      <c r="B29" t="s">
+        <v>63</v>
+      </c>
+      <c r="C29" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" t="s">
+        <v>65</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>0.01</v>
+      </c>
+      <c r="G29" t="s">
+        <v>37</v>
+      </c>
+      <c r="H29">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G30" t="s">
+        <v>174</v>
+      </c>
+      <c r="H30">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G31" t="s">
+        <v>175</v>
+      </c>
+      <c r="H31">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>187</v>
+      </c>
+      <c r="B32" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" t="s">
+        <v>65</v>
+      </c>
+      <c r="D32" t="s">
+        <v>46</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>5</v>
+      </c>
+      <c r="G32" t="s">
+        <v>37</v>
+      </c>
+      <c r="H32">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G33" t="s">
+        <v>174</v>
+      </c>
+      <c r="H33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G34" t="s">
+        <v>175</v>
+      </c>
+      <c r="H34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>188</v>
+      </c>
+      <c r="B35" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" t="s">
+        <v>22</v>
+      </c>
+      <c r="D35" t="s">
+        <v>29</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35">
+        <v>0.01</v>
+      </c>
+      <c r="G35" t="s">
+        <v>37</v>
+      </c>
+      <c r="H35">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G36" t="s">
+        <v>174</v>
+      </c>
+      <c r="H36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G37" t="s">
+        <v>175</v>
+      </c>
+      <c r="H37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G38" t="s">
+        <v>38</v>
+      </c>
+      <c r="H38">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>189</v>
+      </c>
+      <c r="B39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" t="s">
+        <v>29</v>
+      </c>
+      <c r="D39" t="s">
+        <v>46</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39">
+        <v>5</v>
+      </c>
+      <c r="G39" t="s">
+        <v>37</v>
+      </c>
+      <c r="H39">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G40" t="s">
+        <v>174</v>
+      </c>
+      <c r="H40">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G41" t="s">
+        <v>175</v>
+      </c>
+      <c r="H41">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G42" t="s">
+        <v>38</v>
+      </c>
+      <c r="H42">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>190</v>
+      </c>
+      <c r="B43" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" t="s">
+        <v>22</v>
+      </c>
+      <c r="D43" t="s">
+        <v>66</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+      <c r="F43">
+        <v>0.01</v>
+      </c>
+      <c r="G43" t="s">
+        <v>37</v>
+      </c>
+      <c r="H43">
         <v>100</v>
       </c>
-      <c r="J16">
-        <v>0</v>
-      </c>
-      <c r="K16">
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G44" t="s">
+        <v>174</v>
+      </c>
+      <c r="H44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G45" t="s">
+        <v>175</v>
+      </c>
+      <c r="H45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G46" t="s">
+        <v>38</v>
+      </c>
+      <c r="H46">
         <v>300</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>68</v>
-      </c>
-      <c r="B17" t="s">
-        <v>70</v>
-      </c>
-      <c r="C17" t="s">
-        <v>51</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17">
-        <v>10000</v>
-      </c>
-      <c r="H17">
-        <v>5</v>
-      </c>
-      <c r="I17">
-        <v>200</v>
-      </c>
-      <c r="J17">
-        <v>0</v>
-      </c>
-      <c r="K17">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" t="s">
-        <v>77</v>
-      </c>
-      <c r="C18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18">
-        <v>1000</v>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>184</v>
+      </c>
+      <c r="B47" t="s">
+        <v>64</v>
+      </c>
+      <c r="C47" t="s">
+        <v>116</v>
+      </c>
+      <c r="D47" t="s">
+        <v>147</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+      <c r="F47">
+        <v>1</v>
+      </c>
+      <c r="G47" t="s">
+        <v>37</v>
+      </c>
+      <c r="H47">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G48" t="s">
+        <v>174</v>
+      </c>
+      <c r="H48">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G49" t="s">
+        <v>175</v>
+      </c>
+      <c r="H49">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>185</v>
+      </c>
+      <c r="B50" t="s">
+        <v>64</v>
+      </c>
+      <c r="C50" t="s">
+        <v>22</v>
+      </c>
+      <c r="D50" t="s">
+        <v>147</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50">
+        <v>0.01</v>
+      </c>
+      <c r="G50" t="s">
+        <v>37</v>
+      </c>
+      <c r="H50">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G51" t="s">
+        <v>174</v>
+      </c>
+      <c r="H51">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G52" t="s">
+        <v>175</v>
+      </c>
+      <c r="H52">
+        <v>0.7</v>
       </c>
     </row>
   </sheetData>
@@ -1691,10 +1980,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB366907-93DA-4245-BEBF-19818450F8D2}">
-  <dimension ref="A1:J53"/>
+  <dimension ref="A1:H73"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1704,962 +1993,1012 @@
     <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2">
-        <v>100</v>
-      </c>
-      <c r="G2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6">
+        <v>2.35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F9" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9">
+        <v>0.5</v>
+      </c>
+      <c r="H9" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F11" t="s">
+        <v>118</v>
+      </c>
+      <c r="G11">
         <v>0</v>
       </c>
-      <c r="H2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I2">
+      <c r="H11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F12" t="s">
+        <v>125</v>
+      </c>
+      <c r="G12">
+        <v>200</v>
+      </c>
+      <c r="H12" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>136</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F15" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15">
+        <v>2.3519999999999999</v>
+      </c>
+      <c r="H15" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F16" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F17" t="s">
+        <v>35</v>
+      </c>
+      <c r="G17">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F18" t="s">
+        <v>54</v>
+      </c>
+      <c r="G18">
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>149</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E3" t="s">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F19" t="s">
+        <v>55</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F20" t="s">
+        <v>118</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F21" t="s">
+        <v>125</v>
+      </c>
+      <c r="G21">
+        <v>200</v>
+      </c>
+      <c r="H21" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>137</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D22" t="s">
+        <v>128</v>
+      </c>
+      <c r="E22" t="s">
+        <v>28</v>
+      </c>
+      <c r="F22" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F23" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F24" t="s">
         <v>31</v>
       </c>
-      <c r="F3">
-        <v>25</v>
-      </c>
-      <c r="G3">
-        <v>10</v>
-      </c>
-      <c r="H3" t="s">
-        <v>34</v>
-      </c>
-      <c r="I3">
-        <v>2.35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H4" t="s">
+      <c r="G24">
+        <v>2.3540000000000001</v>
+      </c>
+      <c r="H24" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F25" t="s">
+        <v>32</v>
+      </c>
+      <c r="G25">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F26" t="s">
         <v>35</v>
       </c>
-      <c r="I4">
-        <v>0.53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H5" t="s">
-        <v>38</v>
-      </c>
-      <c r="I5">
+      <c r="G26">
         <v>0.05</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I6">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F27" t="s">
+        <v>54</v>
+      </c>
+      <c r="G27">
         <v>0.5</v>
       </c>
-      <c r="J6" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H7" t="s">
-        <v>60</v>
-      </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H8" t="s">
-        <v>132</v>
-      </c>
-      <c r="I8">
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F28" t="s">
+        <v>55</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F29" t="s">
+        <v>118</v>
+      </c>
+      <c r="G29">
         <v>0</v>
       </c>
-      <c r="J8" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H9" t="s">
-        <v>139</v>
-      </c>
-      <c r="I9">
+      <c r="H29" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F30" t="s">
+        <v>125</v>
+      </c>
+      <c r="G30">
         <v>200</v>
       </c>
-      <c r="J9" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>150</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D10" t="s">
-        <v>57</v>
-      </c>
-      <c r="E10" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10">
-        <v>25</v>
-      </c>
-      <c r="G10">
-        <v>10</v>
-      </c>
-      <c r="H10" t="s">
-        <v>34</v>
-      </c>
-      <c r="I10">
-        <v>2.3519999999999999</v>
-      </c>
-      <c r="J10" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H11" t="s">
-        <v>35</v>
-      </c>
-      <c r="I11">
-        <v>0.53</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H12" t="s">
-        <v>38</v>
-      </c>
-      <c r="I12">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H13" t="s">
-        <v>59</v>
-      </c>
-      <c r="I13">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H14" t="s">
-        <v>60</v>
-      </c>
-      <c r="I14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H15" t="s">
-        <v>132</v>
-      </c>
-      <c r="I15">
+      <c r="H30" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>142</v>
+      </c>
+      <c r="B31">
         <v>0</v>
       </c>
-      <c r="J15" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H16" t="s">
-        <v>139</v>
-      </c>
-      <c r="I16">
-        <v>200</v>
-      </c>
-      <c r="J16" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>151</v>
-      </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17" t="s">
-        <v>77</v>
-      </c>
-      <c r="D17" t="s">
-        <v>142</v>
-      </c>
-      <c r="E17" t="s">
-        <v>31</v>
-      </c>
-      <c r="F17">
-        <v>25</v>
-      </c>
-      <c r="G17">
-        <v>10</v>
-      </c>
-      <c r="H17" t="s">
-        <v>34</v>
-      </c>
-      <c r="I17">
-        <v>2.3540000000000001</v>
-      </c>
-      <c r="J17" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H18" t="s">
-        <v>35</v>
-      </c>
-      <c r="I18">
-        <v>0.53</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H19" t="s">
-        <v>38</v>
-      </c>
-      <c r="I19">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H20" t="s">
-        <v>59</v>
-      </c>
-      <c r="I20">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H21" t="s">
-        <v>60</v>
-      </c>
-      <c r="I21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H22" t="s">
-        <v>132</v>
-      </c>
-      <c r="I22">
-        <v>0</v>
-      </c>
-      <c r="J22" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H23" t="s">
-        <v>139</v>
-      </c>
-      <c r="I23">
-        <v>200</v>
-      </c>
-      <c r="J23" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>156</v>
-      </c>
-      <c r="B24">
-        <v>0</v>
-      </c>
-      <c r="C24" t="s">
-        <v>77</v>
-      </c>
-      <c r="D24" t="s">
-        <v>22</v>
-      </c>
-      <c r="E24" t="s">
-        <v>49</v>
-      </c>
-      <c r="F24">
-        <v>1000</v>
-      </c>
-      <c r="G24">
-        <v>0</v>
-      </c>
-      <c r="H24" t="s">
-        <v>50</v>
-      </c>
-      <c r="I24">
+      <c r="C31" t="s">
+        <v>66</v>
+      </c>
+      <c r="D31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E31" t="s">
+        <v>44</v>
+      </c>
+      <c r="F31" t="s">
+        <v>45</v>
+      </c>
+      <c r="G31">
         <f>270/0.1</f>
         <v>2700</v>
       </c>
-      <c r="J24" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>152</v>
-      </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-      <c r="C25" t="s">
-        <v>32</v>
-      </c>
-      <c r="D25" t="s">
-        <v>24</v>
-      </c>
-      <c r="E25" t="s">
+      <c r="H31" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>138</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
         <v>29</v>
       </c>
-      <c r="F25">
-        <v>1000</v>
-      </c>
-      <c r="G25">
-        <v>0</v>
-      </c>
-      <c r="H25" t="s">
-        <v>33</v>
-      </c>
-      <c r="I25">
+      <c r="D32" t="s">
+        <v>21</v>
+      </c>
+      <c r="E32" t="s">
+        <v>26</v>
+      </c>
+      <c r="F32" t="s">
+        <v>30</v>
+      </c>
+      <c r="G32">
         <v>0.4</v>
       </c>
-      <c r="J25" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H26" t="s">
-        <v>115</v>
-      </c>
-      <c r="I26">
+      <c r="H32" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F33" t="s">
+        <v>102</v>
+      </c>
+      <c r="G33">
         <v>300</v>
       </c>
-      <c r="J26" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H27" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="I27">
+      <c r="H33" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F34" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G34">
         <v>20</v>
       </c>
-      <c r="J27" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>160</v>
-      </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
-      <c r="C28" t="s">
-        <v>25</v>
-      </c>
-      <c r="D28" t="s">
-        <v>25</v>
-      </c>
-      <c r="E28" t="s">
-        <v>25</v>
-      </c>
-      <c r="F28">
-        <v>1000</v>
-      </c>
-      <c r="G28">
-        <v>0</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I28" s="2">
+      <c r="H34" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>146</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35" t="s">
+        <v>22</v>
+      </c>
+      <c r="D35" t="s">
+        <v>22</v>
+      </c>
+      <c r="E35" t="s">
+        <v>22</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G35" s="2">
         <v>0.1</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H29" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="I29" s="2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F36" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G36" s="2">
         <v>0.1</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>153</v>
-      </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
-      <c r="C30" t="s">
-        <v>154</v>
-      </c>
-      <c r="D30" t="s">
-        <v>155</v>
-      </c>
-      <c r="E30" t="s">
-        <v>30</v>
-      </c>
-      <c r="F30">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>139</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37" t="s">
+        <v>140</v>
+      </c>
+      <c r="D37" t="s">
+        <v>141</v>
+      </c>
+      <c r="E37" t="s">
+        <v>27</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G37">
         <v>5</v>
       </c>
-      <c r="G30">
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F38" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G38">
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>106</v>
-      </c>
-      <c r="B31">
-        <v>1</v>
-      </c>
-      <c r="C31" t="s">
-        <v>77</v>
-      </c>
-      <c r="D31" t="s">
-        <v>21</v>
-      </c>
-      <c r="E31" t="s">
-        <v>49</v>
-      </c>
-      <c r="F31">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>93</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39" t="s">
+        <v>66</v>
+      </c>
+      <c r="D39" t="s">
+        <v>18</v>
+      </c>
+      <c r="E39" t="s">
+        <v>44</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G39">
         <v>20</v>
       </c>
-      <c r="G31">
-        <v>0</v>
-      </c>
-      <c r="H31" t="s">
-        <v>127</v>
-      </c>
-      <c r="I31" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H32" t="s">
-        <v>50</v>
-      </c>
-      <c r="I32">
-        <v>0</v>
-      </c>
-      <c r="J32" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>107</v>
-      </c>
-      <c r="B33">
-        <v>1</v>
-      </c>
-      <c r="C33" t="s">
-        <v>154</v>
-      </c>
-      <c r="D33" t="s">
-        <v>12</v>
-      </c>
-      <c r="E33" t="s">
-        <v>36</v>
-      </c>
-      <c r="F33">
-        <v>5</v>
-      </c>
-      <c r="G33">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>109</v>
-      </c>
-      <c r="B34">
-        <v>1</v>
-      </c>
-      <c r="C34" t="s">
-        <v>51</v>
-      </c>
-      <c r="D34" t="s">
-        <v>23</v>
-      </c>
-      <c r="E34" t="s">
-        <v>79</v>
-      </c>
-      <c r="F34">
-        <v>1000</v>
-      </c>
-      <c r="G34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>110</v>
-      </c>
-      <c r="B35">
-        <v>1</v>
-      </c>
-      <c r="C35" t="s">
-        <v>51</v>
-      </c>
-      <c r="D35" t="s">
-        <v>78</v>
-      </c>
-      <c r="E35" t="s">
-        <v>80</v>
-      </c>
-      <c r="F35">
-        <v>1000</v>
-      </c>
-      <c r="G35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>111</v>
-      </c>
-      <c r="B36">
-        <v>0</v>
-      </c>
-      <c r="C36" t="s">
-        <v>77</v>
-      </c>
-      <c r="D36" t="s">
-        <v>12</v>
-      </c>
-      <c r="E36" t="s">
-        <v>36</v>
-      </c>
-      <c r="F36">
-        <v>4</v>
-      </c>
-      <c r="G36">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>61</v>
-      </c>
-      <c r="B37">
-        <v>0</v>
-      </c>
-      <c r="C37" t="s">
-        <v>77</v>
-      </c>
-      <c r="D37" t="s">
-        <v>61</v>
-      </c>
-      <c r="E37" t="s">
-        <v>62</v>
-      </c>
-      <c r="F37">
-        <v>4</v>
-      </c>
-      <c r="G37">
-        <v>0</v>
-      </c>
-      <c r="H37" t="s">
-        <v>33</v>
-      </c>
-      <c r="I37">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H38" t="s">
-        <v>63</v>
-      </c>
-      <c r="I38">
-        <v>2</v>
-      </c>
-      <c r="J38" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>64</v>
-      </c>
-      <c r="B39">
-        <v>1</v>
-      </c>
-      <c r="C39" t="s">
-        <v>130</v>
-      </c>
-      <c r="D39" t="s">
-        <v>64</v>
-      </c>
-      <c r="E39" t="s">
-        <v>67</v>
-      </c>
-      <c r="F39">
-        <v>15</v>
-      </c>
-      <c r="G39">
-        <v>0</v>
-      </c>
-      <c r="H39" t="s">
-        <v>42</v>
-      </c>
-      <c r="I39">
-        <v>6</v>
-      </c>
-      <c r="J39" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H40" t="s">
-        <v>127</v>
-      </c>
-      <c r="I40" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>65</v>
-      </c>
-      <c r="B41">
-        <v>1</v>
-      </c>
-      <c r="C41" t="s">
-        <v>130</v>
-      </c>
-      <c r="D41" t="s">
-        <v>65</v>
-      </c>
-      <c r="E41" t="s">
-        <v>67</v>
-      </c>
-      <c r="F41">
-        <v>35</v>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F40" t="s">
+        <v>113</v>
+      </c>
+      <c r="G40" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F41" t="s">
+        <v>45</v>
       </c>
       <c r="G41">
         <v>0</v>
       </c>
       <c r="H41" t="s">
-        <v>42</v>
-      </c>
-      <c r="I41">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>94</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42" t="s">
+        <v>140</v>
+      </c>
+      <c r="D42" t="s">
+        <v>10</v>
+      </c>
+      <c r="E42" t="s">
+        <v>33</v>
+      </c>
+      <c r="F42" t="s">
+        <v>13</v>
+      </c>
+      <c r="G42">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F43" t="s">
+        <v>14</v>
+      </c>
+      <c r="G43">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>96</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44" t="s">
+        <v>46</v>
+      </c>
+      <c r="D44" t="s">
+        <v>20</v>
+      </c>
+      <c r="E44" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>97</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45" t="s">
+        <v>46</v>
+      </c>
+      <c r="D45" t="s">
+        <v>67</v>
+      </c>
+      <c r="E45" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>98</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
+      <c r="C46" t="s">
+        <v>66</v>
+      </c>
+      <c r="D46" t="s">
+        <v>10</v>
+      </c>
+      <c r="E46" t="s">
+        <v>33</v>
+      </c>
+      <c r="F46" t="s">
+        <v>13</v>
+      </c>
+      <c r="G46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F47" t="s">
+        <v>14</v>
+      </c>
+      <c r="G47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>56</v>
+      </c>
+      <c r="B48">
+        <v>0</v>
+      </c>
+      <c r="C48" t="s">
+        <v>66</v>
+      </c>
+      <c r="D48" t="s">
+        <v>56</v>
+      </c>
+      <c r="E48" t="s">
+        <v>57</v>
+      </c>
+      <c r="F48" t="s">
+        <v>13</v>
+      </c>
+      <c r="G48">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F49" t="s">
+        <v>14</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F50" t="s">
+        <v>30</v>
+      </c>
+      <c r="G50">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F51" t="s">
+        <v>58</v>
+      </c>
+      <c r="G51">
+        <v>2</v>
+      </c>
+      <c r="H51" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>59</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52" t="s">
+        <v>116</v>
+      </c>
+      <c r="D52" t="s">
+        <v>59</v>
+      </c>
+      <c r="E52" t="s">
+        <v>62</v>
+      </c>
+      <c r="F52" t="s">
+        <v>150</v>
+      </c>
+      <c r="G52">
+        <v>15</v>
+      </c>
+      <c r="H52" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F53" t="s">
+        <v>39</v>
+      </c>
+      <c r="G53">
         <v>6</v>
       </c>
-      <c r="J41" t="s">
+      <c r="H53" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F54" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H42" t="s">
-        <v>127</v>
-      </c>
-      <c r="I42" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>66</v>
-      </c>
-      <c r="B43">
+      <c r="G54" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>60</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="C55" t="s">
+        <v>116</v>
+      </c>
+      <c r="D55" t="s">
+        <v>60</v>
+      </c>
+      <c r="E55" t="s">
+        <v>62</v>
+      </c>
+      <c r="F55" t="s">
+        <v>150</v>
+      </c>
+      <c r="G55">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F56" t="s">
+        <v>39</v>
+      </c>
+      <c r="G56">
+        <v>6</v>
+      </c>
+      <c r="H56" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F57" t="s">
+        <v>113</v>
+      </c>
+      <c r="G57" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>61</v>
+      </c>
+      <c r="B58">
         <v>0</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C58" t="s">
+        <v>116</v>
+      </c>
+      <c r="D58" t="s">
+        <v>61</v>
+      </c>
+      <c r="E58" t="s">
+        <v>62</v>
+      </c>
+      <c r="F58" t="s">
+        <v>39</v>
+      </c>
+      <c r="G58">
+        <v>6</v>
+      </c>
+      <c r="H58" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F59" t="s">
+        <v>150</v>
+      </c>
+      <c r="G59">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F60" t="s">
+        <v>113</v>
+      </c>
+      <c r="G60" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>145</v>
+      </c>
+      <c r="B61">
+        <v>1</v>
+      </c>
+      <c r="C61" t="s">
+        <v>65</v>
+      </c>
+      <c r="D61" t="s">
+        <v>74</v>
+      </c>
+      <c r="E61" t="s">
+        <v>65</v>
+      </c>
+      <c r="F61" t="s">
+        <v>30</v>
+      </c>
+      <c r="G61">
+        <v>0.8</v>
+      </c>
+      <c r="H61" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>144</v>
+      </c>
+      <c r="B62">
+        <v>1</v>
+      </c>
+      <c r="C62" t="s">
+        <v>133</v>
+      </c>
+      <c r="D62" t="s">
+        <v>131</v>
+      </c>
+      <c r="E62" t="s">
+        <v>132</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G62" s="2">
+        <v>3</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>143</v>
+      </c>
+      <c r="B63">
+        <v>1</v>
+      </c>
+      <c r="C63" t="s">
+        <v>147</v>
+      </c>
+      <c r="D63" t="s">
+        <v>75</v>
+      </c>
+      <c r="E63" t="s">
+        <v>76</v>
+      </c>
+      <c r="F63" t="s">
+        <v>150</v>
+      </c>
+      <c r="G63">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F64" t="s">
+        <v>152</v>
+      </c>
+      <c r="G64">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F65" t="s">
+        <v>30</v>
+      </c>
+      <c r="G65">
+        <v>0.8</v>
+      </c>
+      <c r="H65" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F66" t="s">
+        <v>108</v>
+      </c>
+      <c r="G66">
+        <v>6</v>
+      </c>
+      <c r="H66" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F67" t="s">
+        <v>193</v>
+      </c>
+      <c r="G67">
+        <v>1.3</v>
+      </c>
+      <c r="H67" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F68" t="s">
+        <v>194</v>
+      </c>
+      <c r="G68">
+        <v>1.3</v>
+      </c>
+      <c r="H68" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F69" t="s">
+        <v>129</v>
+      </c>
+      <c r="G69">
+        <v>1</v>
+      </c>
+      <c r="H69" t="s">
         <v>130</v>
       </c>
-      <c r="D43" t="s">
-        <v>66</v>
-      </c>
-      <c r="E43" t="s">
-        <v>67</v>
-      </c>
-      <c r="F43">
-        <v>20</v>
-      </c>
-      <c r="G43">
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>95</v>
+      </c>
+      <c r="B70">
+        <v>1</v>
+      </c>
+      <c r="C70" t="s">
+        <v>116</v>
+      </c>
+      <c r="D70" t="s">
+        <v>117</v>
+      </c>
+      <c r="E70" t="s">
+        <v>90</v>
+      </c>
+      <c r="F70" t="s">
+        <v>39</v>
+      </c>
+      <c r="G70">
+        <v>0.7</v>
+      </c>
+      <c r="H70" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F71" t="s">
+        <v>150</v>
+      </c>
+      <c r="G71">
+        <v>5</v>
+      </c>
+      <c r="H71" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>148</v>
+      </c>
+      <c r="B72">
         <v>0</v>
       </c>
-      <c r="H43" t="s">
-        <v>42</v>
-      </c>
-      <c r="I43">
-        <v>6</v>
-      </c>
-      <c r="J43" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H44" t="s">
-        <v>127</v>
-      </c>
-      <c r="I44" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>159</v>
-      </c>
-      <c r="B45">
-        <v>1</v>
-      </c>
-      <c r="C45" t="s">
+      <c r="C72" t="s">
+        <v>147</v>
+      </c>
+      <c r="D72" t="s">
         <v>70</v>
       </c>
-      <c r="D45" t="s">
-        <v>85</v>
-      </c>
-      <c r="E45" t="s">
-        <v>70</v>
-      </c>
-      <c r="F45">
+      <c r="E72" t="s">
+        <v>71</v>
+      </c>
+      <c r="F72" t="s">
+        <v>150</v>
+      </c>
+      <c r="G72">
         <v>1000</v>
       </c>
-      <c r="G45">
-        <v>0</v>
-      </c>
-      <c r="H45" t="s">
-        <v>33</v>
-      </c>
-      <c r="I45">
-        <v>0.8</v>
-      </c>
-      <c r="J45" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>158</v>
-      </c>
-      <c r="B46">
-        <v>1</v>
-      </c>
-      <c r="C46" t="s">
-        <v>147</v>
-      </c>
-      <c r="D46" t="s">
-        <v>145</v>
-      </c>
-      <c r="E46" t="s">
-        <v>146</v>
-      </c>
-      <c r="F46">
-        <v>1000</v>
-      </c>
-      <c r="G46">
-        <v>0</v>
-      </c>
-      <c r="H46" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I46" s="2">
-        <v>3</v>
-      </c>
-      <c r="J46" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>157</v>
-      </c>
-      <c r="B47">
-        <v>1</v>
-      </c>
-      <c r="C47" t="s">
-        <v>161</v>
-      </c>
-      <c r="D47" t="s">
-        <v>86</v>
-      </c>
-      <c r="E47" t="s">
-        <v>87</v>
-      </c>
-      <c r="F47">
-        <v>1.3</v>
-      </c>
-      <c r="G47">
-        <v>1.3</v>
-      </c>
-      <c r="H47" t="s">
-        <v>33</v>
-      </c>
-      <c r="I47">
-        <v>0.8</v>
-      </c>
-      <c r="J47" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H48" t="s">
-        <v>121</v>
-      </c>
-      <c r="I48">
-        <v>6</v>
-      </c>
-      <c r="J48" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H49" t="s">
-        <v>124</v>
-      </c>
-      <c r="I49">
-        <v>1.3</v>
-      </c>
-      <c r="J49" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H50" t="s">
-        <v>63</v>
-      </c>
-      <c r="I50">
-        <v>1.3</v>
-      </c>
-      <c r="J50" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H51" t="s">
-        <v>143</v>
-      </c>
-      <c r="I51">
-        <v>1</v>
-      </c>
-      <c r="J51" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>108</v>
-      </c>
-      <c r="B52">
-        <v>1</v>
-      </c>
-      <c r="C52" t="s">
-        <v>130</v>
-      </c>
-      <c r="D52" t="s">
-        <v>131</v>
-      </c>
-      <c r="E52" t="s">
-        <v>103</v>
-      </c>
-      <c r="F52">
-        <v>5</v>
-      </c>
-      <c r="G52">
-        <v>0</v>
-      </c>
-      <c r="H52" t="s">
-        <v>42</v>
-      </c>
-      <c r="I52">
-        <v>0.7</v>
-      </c>
-      <c r="J52" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>162</v>
-      </c>
-      <c r="B53">
-        <v>0</v>
-      </c>
-      <c r="C53" t="s">
-        <v>161</v>
-      </c>
-      <c r="D53" t="s">
-        <v>81</v>
-      </c>
-      <c r="E53" t="s">
-        <v>82</v>
-      </c>
-      <c r="F53">
-        <v>1000</v>
-      </c>
-      <c r="G53">
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F73" t="s">
+        <v>152</v>
+      </c>
+      <c r="G73">
         <v>0</v>
       </c>
     </row>
@@ -2670,11 +3009,294 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B173308-94D5-4307-9C97-06EC5F416B49}">
+  <dimension ref="A1:D24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C2">
+        <v>2E-3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C3">
+        <v>0.995</v>
+      </c>
+      <c r="D3" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>201</v>
+      </c>
+      <c r="C4">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>153</v>
+      </c>
+      <c r="C5">
+        <v>5.63</v>
+      </c>
+      <c r="D5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>154</v>
+      </c>
+      <c r="C6">
+        <v>1E-3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" t="s">
+        <v>153</v>
+      </c>
+      <c r="C7">
+        <v>1000</v>
+      </c>
+      <c r="D7" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C8">
+        <v>1E-3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" t="s">
+        <v>153</v>
+      </c>
+      <c r="C9">
+        <v>900</v>
+      </c>
+      <c r="D9" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>154</v>
+      </c>
+      <c r="C10">
+        <v>2.5999999999999999E-3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>155</v>
+      </c>
+      <c r="C11">
+        <v>419</v>
+      </c>
+      <c r="D11" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>156</v>
+      </c>
+      <c r="C12">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>153</v>
+      </c>
+      <c r="C13">
+        <v>0.84</v>
+      </c>
+      <c r="D13" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>157</v>
+      </c>
+      <c r="C14">
+        <v>40</v>
+      </c>
+      <c r="D14" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>158</v>
+      </c>
+      <c r="C15">
+        <v>2.34</v>
+      </c>
+      <c r="D15" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>155</v>
+      </c>
+      <c r="C16">
+        <v>0.41899999999999998</v>
+      </c>
+      <c r="D16" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>159</v>
+      </c>
+      <c r="C17">
+        <f>273+15</f>
+        <v>288</v>
+      </c>
+      <c r="D17" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>160</v>
+      </c>
+      <c r="C18">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="D18" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>161</v>
+      </c>
+      <c r="C19">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>162</v>
+      </c>
+      <c r="C20">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>163</v>
+      </c>
+      <c r="C21">
+        <v>1.27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>164</v>
+      </c>
+      <c r="C22">
+        <v>500</v>
+      </c>
+      <c r="D22" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" t="s">
+        <v>172</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98F6EB10-AB47-4D11-878D-7EA50574CBA2}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2685,183 +3307,173 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C1" t="s">
-        <v>10</v>
+      <c r="A1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B2">
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B3">
         <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B4">
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="B5">
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="B6">
         <v>0.04</v>
       </c>
       <c r="C6" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B7" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="C7" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="B8">
         <v>0.05</v>
       </c>
       <c r="C8" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="B9">
         <v>-1</v>
       </c>
       <c r="C9" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="B10">
         <v>-1</v>
       </c>
       <c r="C10" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C11" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="B12" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="C12" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="B13">
         <v>0.5</v>
       </c>
       <c r="C13" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>94</v>
-      </c>
-      <c r="B14" t="s">
-        <v>51</v>
-      </c>
-      <c r="C14" t="s">
-        <v>95</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3E6B22F-D4D7-489D-AE2A-F030E504A301}">
   <dimension ref="A1:C290"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -6048,7 +6660,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB42B24B-1FF3-4D04-ABC3-37C8B4C6ACE7}">
   <dimension ref="A1:C290"/>
   <sheetViews>
@@ -6058,13 +6670,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -9461,18 +10073,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9495,18 +10107,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78762D46-3C96-44E4-BFC9-B88DF736E950}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B20FA7CB-4913-4ED5-B2A6-1FAA15DCEB4D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78762D46-3C96-44E4-BFC9-B88DF736E950}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
-split injection well into pump+watersink -updated example case
</commit_message>
<xml_diff>
--- a/examples/data_example2.xlsx
+++ b/examples/data_example2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsven\code\OffshoreEnergySystem_OOGESO\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE6057C8-59D7-4700-97CF-103A9B030E01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84A002D5-CF77-4FFC-AE46-223AEDFEAB5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5064" yWindow="3516" windowWidth="23040" windowHeight="12996" activeTab="3" xr2:uid="{67DC4D86-39E4-4DA3-B21D-C0F42277600B}"/>
+    <workbookView xWindow="5064" yWindow="3516" windowWidth="23040" windowHeight="12996" xr2:uid="{67DC4D86-39E4-4DA3-B21D-C0F42277600B}"/>
   </bookViews>
   <sheets>
     <sheet name="node" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="212">
   <si>
     <t>id</t>
   </si>
@@ -269,9 +269,6 @@
     <t>water injection</t>
   </si>
   <si>
-    <t>well_injection</t>
-  </si>
-  <si>
     <t>wellstream</t>
   </si>
   <si>
@@ -365,9 +362,6 @@
     <t>pump efficiency</t>
   </si>
   <si>
-    <t>injectionpressure</t>
-  </si>
-  <si>
     <t>MPa - at least as much as production well pressure</t>
   </si>
   <si>
@@ -660,6 +654,27 @@
   </si>
   <si>
     <t>kg/Sm3 - SSB 2016 report</t>
+  </si>
+  <si>
+    <t>pump_water</t>
+  </si>
+  <si>
+    <t>injectionwell</t>
+  </si>
+  <si>
+    <t>water injection pump</t>
+  </si>
+  <si>
+    <t>w3</t>
+  </si>
+  <si>
+    <t>XXXpressure</t>
+  </si>
+  <si>
+    <t>maxdeviation_pressure.water.in</t>
+  </si>
+  <si>
+    <t>maxdeviation_pressure.wellstream.in</t>
   </si>
 </sst>
 </file>
@@ -1028,17 +1043,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{052C0DB0-0590-4B7A-AC1E-E28475B8C302}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.33203125" customWidth="1"/>
-    <col min="3" max="3" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="14.33203125" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
   </cols>
@@ -1051,10 +1066,10 @@
         <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>8</v>
@@ -1066,7 +1081,7 @@
         <v>2</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -1085,7 +1100,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F3">
         <v>-1</v>
@@ -1099,7 +1114,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F4">
         <v>2</v>
@@ -1113,7 +1128,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F5">
         <v>2</v>
@@ -1129,6 +1144,12 @@
       <c r="A6" t="s">
         <v>22</v>
       </c>
+      <c r="C6" t="s">
+        <v>211</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
       <c r="F6">
         <v>0</v>
       </c>
@@ -1169,7 +1190,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>147</v>
+        <v>205</v>
       </c>
       <c r="F9">
         <v>-1</v>
@@ -1183,36 +1204,50 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>145</v>
       </c>
       <c r="C10" t="s">
-        <v>195</v>
+        <v>210</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>198</v>
-      </c>
-      <c r="F10">
-        <v>-1.2</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="H10" t="s">
-        <v>16</v>
+        <v>196</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>46</v>
+      </c>
       <c r="C11" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D11">
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>198</v>
+        <v>196</v>
+      </c>
+      <c r="F11">
+        <v>-1.2</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>194</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -1223,10 +1258,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00A70904-C380-433D-9493-9658C938F213}">
-  <dimension ref="A1:H52"/>
+  <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1259,15 +1294,15 @@
         <v>36</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -1276,7 +1311,7 @@
         <v>66</v>
       </c>
       <c r="D2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -1293,7 +1328,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="H3">
         <v>1E-3</v>
@@ -1309,7 +1344,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
@@ -1335,7 +1370,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="H6">
         <v>1E-3</v>
@@ -1351,7 +1386,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
@@ -1360,7 +1395,7 @@
         <v>66</v>
       </c>
       <c r="D8" t="s">
-        <v>147</v>
+        <v>205</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -1377,7 +1412,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G9" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="H9">
         <v>1E-3</v>
@@ -1393,7 +1428,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B11" t="s">
         <v>4</v>
@@ -1419,7 +1454,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G12" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="H12">
         <v>1E-3</v>
@@ -1435,7 +1470,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B14" t="s">
         <v>4</v>
@@ -1461,7 +1496,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G15" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="H15">
         <v>1E-3</v>
@@ -1477,7 +1512,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B17" t="s">
         <v>4</v>
@@ -1486,7 +1521,7 @@
         <v>66</v>
       </c>
       <c r="D17" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -1503,7 +1538,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G18" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="H18">
         <v>1E-3</v>
@@ -1519,7 +1554,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B20" t="s">
         <v>35</v>
@@ -1528,7 +1563,7 @@
         <v>66</v>
       </c>
       <c r="D20" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -1542,7 +1577,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B21" t="s">
         <v>35</v>
@@ -1565,16 +1600,16 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C22" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D22" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E22">
         <v>1</v>
@@ -1591,7 +1626,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G23" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H23">
         <v>6</v>
@@ -1599,7 +1634,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G24" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H24">
         <v>6</v>
@@ -1607,13 +1642,13 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C25" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D25" t="s">
         <v>22</v>
@@ -1633,7 +1668,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G26" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H26">
         <v>6</v>
@@ -1641,7 +1676,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G27" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H27">
         <v>6</v>
@@ -1649,7 +1684,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G28" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H28">
         <v>0</v>
@@ -1657,7 +1692,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B29" t="s">
         <v>63</v>
@@ -1683,7 +1718,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G30" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H30">
         <v>0.3</v>
@@ -1691,7 +1726,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G31" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H31">
         <v>0.3</v>
@@ -1699,7 +1734,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B32" t="s">
         <v>63</v>
@@ -1725,7 +1760,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G33" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H33">
         <v>5</v>
@@ -1733,7 +1768,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G34" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H34">
         <v>3</v>
@@ -1741,7 +1776,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B35" t="s">
         <v>5</v>
@@ -1767,7 +1802,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G36" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H36">
         <v>2</v>
@@ -1775,7 +1810,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G37" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H37">
         <v>2</v>
@@ -1791,7 +1826,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B39" t="s">
         <v>5</v>
@@ -1817,7 +1852,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G40" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H40">
         <v>10</v>
@@ -1825,7 +1860,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G41" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H41">
         <v>6</v>
@@ -1841,7 +1876,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B43" t="s">
         <v>5</v>
@@ -1867,7 +1902,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G44" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H44">
         <v>2</v>
@@ -1875,7 +1910,7 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G45" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H45">
         <v>2</v>
@@ -1891,16 +1926,16 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B47" t="s">
         <v>64</v>
       </c>
       <c r="C47" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D47" t="s">
-        <v>147</v>
+        <v>205</v>
       </c>
       <c r="E47">
         <v>1</v>
@@ -1917,7 +1952,7 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G48" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H48">
         <v>0.7</v>
@@ -1925,7 +1960,7 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G49" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H49">
         <v>0.7</v>
@@ -1933,7 +1968,7 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B50" t="s">
         <v>64</v>
@@ -1942,7 +1977,7 @@
         <v>22</v>
       </c>
       <c r="D50" t="s">
-        <v>147</v>
+        <v>205</v>
       </c>
       <c r="E50">
         <v>1</v>
@@ -1959,7 +1994,7 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G51" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H51">
         <v>0.7</v>
@@ -1967,10 +2002,52 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G52" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H52">
         <v>0.7</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>208</v>
+      </c>
+      <c r="B53" t="s">
+        <v>64</v>
+      </c>
+      <c r="C53" t="s">
+        <v>205</v>
+      </c>
+      <c r="D53" t="s">
+        <v>145</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="F53">
+        <v>0.01</v>
+      </c>
+      <c r="G53" t="s">
+        <v>37</v>
+      </c>
+      <c r="H53">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G54" t="s">
+        <v>172</v>
+      </c>
+      <c r="H54">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G55" t="s">
+        <v>173</v>
+      </c>
+      <c r="H55">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1980,10 +2057,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB366907-93DA-4245-BEBF-19818450F8D2}">
-  <dimension ref="A1:H73"/>
+  <dimension ref="A1:H75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="G62" sqref="G62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2014,10 +2091,10 @@
         <v>25</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>8</v>
@@ -2056,7 +2133,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -2117,7 +2194,7 @@
         <v>0.5</v>
       </c>
       <c r="H9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -2130,29 +2207,29 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G11">
         <v>0</v>
       </c>
       <c r="H11" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G12">
         <v>200</v>
       </c>
       <c r="H12" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -2189,7 +2266,7 @@
         <v>2.3519999999999999</v>
       </c>
       <c r="H15" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -2226,29 +2303,29 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F20" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G20">
         <v>0</v>
       </c>
       <c r="H20" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F21" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G21">
         <v>200</v>
       </c>
       <c r="H21" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -2257,7 +2334,7 @@
         <v>66</v>
       </c>
       <c r="D22" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E22" t="s">
         <v>28</v>
@@ -2285,7 +2362,7 @@
         <v>2.3540000000000001</v>
       </c>
       <c r="H24" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
@@ -2322,29 +2399,29 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F29" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G29">
         <v>0</v>
       </c>
       <c r="H29" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F30" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G30">
         <v>200</v>
       </c>
       <c r="H30" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -2366,12 +2443,12 @@
         <v>2700</v>
       </c>
       <c r="H31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -2392,34 +2469,34 @@
         <v>0.4</v>
       </c>
       <c r="H32" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F33" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G33">
         <v>300</v>
       </c>
       <c r="H33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F34" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G34">
         <v>20</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -2442,7 +2519,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F36" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G36" s="2">
         <v>0.1</v>
@@ -2450,16 +2527,16 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>137</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37" t="s">
+        <v>138</v>
+      </c>
+      <c r="D37" t="s">
         <v>139</v>
-      </c>
-      <c r="B37">
-        <v>1</v>
-      </c>
-      <c r="C37" t="s">
-        <v>140</v>
-      </c>
-      <c r="D37" t="s">
-        <v>141</v>
       </c>
       <c r="E37" t="s">
         <v>27</v>
@@ -2481,7 +2558,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B39">
         <v>1</v>
@@ -2504,7 +2581,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F40" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G40" t="s">
         <v>11</v>
@@ -2518,18 +2595,18 @@
         <v>0</v>
       </c>
       <c r="H41" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B42">
         <v>1</v>
       </c>
       <c r="C42" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D42" t="s">
         <v>10</v>
@@ -2554,7 +2631,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -2571,7 +2648,7 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B45">
         <v>1</v>
@@ -2588,7 +2665,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -2664,7 +2741,7 @@
         <v>2</v>
       </c>
       <c r="H51" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
@@ -2675,7 +2752,7 @@
         <v>1</v>
       </c>
       <c r="C52" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D52" t="s">
         <v>59</v>
@@ -2684,13 +2761,13 @@
         <v>62</v>
       </c>
       <c r="F52" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G52">
         <v>15</v>
       </c>
       <c r="H52" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
@@ -2701,12 +2778,12 @@
         <v>6</v>
       </c>
       <c r="H53" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F54" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G54" t="s">
         <v>43</v>
@@ -2720,7 +2797,7 @@
         <v>1</v>
       </c>
       <c r="C55" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D55" t="s">
         <v>60</v>
@@ -2729,7 +2806,7 @@
         <v>62</v>
       </c>
       <c r="F55" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G55">
         <v>35</v>
@@ -2743,12 +2820,12 @@
         <v>6</v>
       </c>
       <c r="H56" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F57" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G57" t="s">
         <v>43</v>
@@ -2762,7 +2839,7 @@
         <v>0</v>
       </c>
       <c r="C58" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D58" t="s">
         <v>61</v>
@@ -2777,12 +2854,12 @@
         <v>6</v>
       </c>
       <c r="H58" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F59" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G59">
         <v>20</v>
@@ -2790,7 +2867,7 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F60" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G60" t="s">
         <v>43</v>
@@ -2798,7 +2875,7 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B61">
         <v>1</v>
@@ -2819,24 +2896,24 @@
         <v>0.8</v>
       </c>
       <c r="H61" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B62">
         <v>1</v>
       </c>
       <c r="C62" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D62" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E62" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F62" s="2" t="s">
         <v>30</v>
@@ -2845,38 +2922,38 @@
         <v>3</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B63">
         <v>1</v>
       </c>
       <c r="C63" t="s">
-        <v>147</v>
+        <v>205</v>
       </c>
       <c r="D63" t="s">
-        <v>75</v>
+        <v>207</v>
       </c>
       <c r="E63" t="s">
-        <v>76</v>
+        <v>205</v>
       </c>
       <c r="F63" t="s">
-        <v>150</v>
+        <v>13</v>
       </c>
       <c r="G63">
-        <v>1.3</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F64" t="s">
-        <v>152</v>
+        <v>14</v>
       </c>
       <c r="G64">
-        <v>1.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.3">
@@ -2887,118 +2964,149 @@
         <v>0.8</v>
       </c>
       <c r="H65" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F66" t="s">
-        <v>108</v>
+        <v>127</v>
       </c>
       <c r="G66">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H66" t="s">
-        <v>109</v>
+        <v>128</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>206</v>
+      </c>
+      <c r="B67">
+        <v>1</v>
+      </c>
+      <c r="C67" t="s">
+        <v>145</v>
+      </c>
+      <c r="D67" t="s">
+        <v>75</v>
+      </c>
+      <c r="E67" t="s">
+        <v>71</v>
+      </c>
       <c r="F67" t="s">
-        <v>193</v>
+        <v>148</v>
       </c>
       <c r="G67">
         <v>1.3</v>
       </c>
-      <c r="H67" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F68" t="s">
-        <v>194</v>
+        <v>150</v>
       </c>
       <c r="G68">
         <v>1.3</v>
       </c>
-      <c r="H68" t="s">
-        <v>112</v>
-      </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F69" t="s">
-        <v>129</v>
+        <v>209</v>
       </c>
       <c r="G69">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H69" t="s">
-        <v>130</v>
+        <v>107</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
-        <v>95</v>
-      </c>
-      <c r="B70">
-        <v>1</v>
-      </c>
-      <c r="C70" t="s">
-        <v>116</v>
-      </c>
-      <c r="D70" t="s">
-        <v>117</v>
-      </c>
-      <c r="E70" t="s">
-        <v>90</v>
-      </c>
       <c r="F70" t="s">
-        <v>39</v>
+        <v>191</v>
       </c>
       <c r="G70">
-        <v>0.7</v>
+        <v>1.3</v>
       </c>
       <c r="H70" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F71" t="s">
-        <v>150</v>
+        <v>192</v>
       </c>
       <c r="G71">
-        <v>5</v>
+        <v>1.3</v>
       </c>
       <c r="H71" t="s">
-        <v>151</v>
+        <v>110</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>148</v>
+        <v>94</v>
       </c>
       <c r="B72">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C72" t="s">
-        <v>147</v>
+        <v>114</v>
       </c>
       <c r="D72" t="s">
-        <v>70</v>
+        <v>115</v>
       </c>
       <c r="E72" t="s">
-        <v>71</v>
+        <v>89</v>
       </c>
       <c r="F72" t="s">
-        <v>150</v>
+        <v>39</v>
       </c>
       <c r="G72">
-        <v>1000</v>
+        <v>0.7</v>
+      </c>
+      <c r="H72" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F73" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="G73">
+        <v>5</v>
+      </c>
+      <c r="H73" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>146</v>
+      </c>
+      <c r="B74">
+        <v>0</v>
+      </c>
+      <c r="C74" t="s">
+        <v>145</v>
+      </c>
+      <c r="D74" t="s">
+        <v>70</v>
+      </c>
+      <c r="E74" t="s">
+        <v>71</v>
+      </c>
+      <c r="F74" t="s">
+        <v>148</v>
+      </c>
+      <c r="G74">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F75" t="s">
+        <v>150</v>
+      </c>
+      <c r="G75">
         <v>0</v>
       </c>
     </row>
@@ -3012,15 +3120,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B173308-94D5-4307-9C97-06EC5F416B49}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="56.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -3028,71 +3137,71 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C2">
         <v>2E-3</v>
       </c>
       <c r="D2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C3">
         <v>0.995</v>
       </c>
       <c r="D3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C4">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="D4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C5">
         <v>5.63</v>
       </c>
       <c r="D5" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C6">
         <v>1E-3</v>
       </c>
       <c r="D6" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -3100,24 +3209,24 @@
         <v>64</v>
       </c>
       <c r="B7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C7">
         <v>1000</v>
       </c>
       <c r="D7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C8">
         <v>1E-3</v>
       </c>
       <c r="D8" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -3125,40 +3234,40 @@
         <v>63</v>
       </c>
       <c r="B9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C9">
         <v>900</v>
       </c>
       <c r="D9" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C10">
         <v>2.5999999999999999E-3</v>
       </c>
       <c r="D10" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C11">
         <v>419</v>
       </c>
       <c r="D11" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C12">
         <v>0.02</v>
@@ -3169,74 +3278,74 @@
         <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C13">
         <v>0.84</v>
       </c>
       <c r="D13" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C14">
         <v>40</v>
       </c>
       <c r="D14" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C15">
         <v>2.34</v>
       </c>
       <c r="D15" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C16">
         <v>0.41899999999999998</v>
       </c>
       <c r="D16" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C17">
         <f>273+15</f>
         <v>288</v>
       </c>
       <c r="D17" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C18">
         <v>0.10100000000000001</v>
       </c>
       <c r="D18" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C19">
         <v>0.6</v>
@@ -3244,7 +3353,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C20">
         <v>0.9</v>
@@ -3252,7 +3361,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C21">
         <v>1.27</v>
@@ -3260,13 +3369,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C22">
         <v>500</v>
       </c>
       <c r="D22" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -3274,7 +3383,7 @@
         <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -3282,7 +3391,7 @@
         <v>35</v>
       </c>
       <c r="D24" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -3303,15 +3412,15 @@
   <cols>
     <col min="1" max="1" width="21.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="57.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>8</v>
@@ -3325,7 +3434,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -3336,7 +3445,7 @@
         <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -3352,24 +3461,24 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B5">
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B6">
         <v>0.04</v>
       </c>
       <c r="C6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -3396,57 +3505,57 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B9">
         <v>-1</v>
       </c>
       <c r="C9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B10">
         <v>-1</v>
       </c>
       <c r="C10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B11" t="s">
         <v>46</v>
       </c>
       <c r="C11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" t="s">
+        <v>87</v>
+      </c>
+      <c r="C12" t="s">
         <v>84</v>
-      </c>
-      <c r="B12" t="s">
-        <v>88</v>
-      </c>
-      <c r="C12" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B13">
         <v>0.5</v>
       </c>
       <c r="C13" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -9864,6 +9973,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010068757AD89D0841429F5831BBC6267AC1" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3e521892cf07d8fee7d1fab9fe3aaa83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="78e0c6f3-9112-4e2d-9710-8a99a0c0b95c" xmlns:ns4="53f6e7f0-9e34-4545-9b50-e54ccadfb78a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3ffc55c83d6521c05fad87c69f289641" ns3:_="" ns4:_="">
     <xsd:import namespace="78e0c6f3-9112-4e2d-9710-8a99a0c0b95c"/>
@@ -10072,22 +10196,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78762D46-3C96-44E4-BFC9-B88DF736E950}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B20FA7CB-4913-4ED5-B2A6-1FAA15DCEB4D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1016DCAE-9D9F-40DE-A38A-1587953D2A7E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10104,21 +10230,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B20FA7CB-4913-4ED5-B2A6-1FAA15DCEB4D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78762D46-3C96-44E4-BFC9-B88DF736E950}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
including wellstream transport (pipe pressure drop and pump)
</commit_message>
<xml_diff>
--- a/examples/data_example2.xlsx
+++ b/examples/data_example2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsven\code\OffshoreEnergySystem_OOGESO\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84A002D5-CF77-4FFC-AE46-223AEDFEAB5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{539BDF98-70EB-4CFD-AB63-F7B0D873B851}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5064" yWindow="3516" windowWidth="23040" windowHeight="12996" xr2:uid="{67DC4D86-39E4-4DA3-B21D-C0F42277600B}"/>
+    <workbookView xWindow="5064" yWindow="3516" windowWidth="25092" windowHeight="12996" activeTab="2" xr2:uid="{67DC4D86-39E4-4DA3-B21D-C0F42277600B}"/>
   </bookViews>
   <sheets>
     <sheet name="node" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="230">
   <si>
     <t>id</t>
   </si>
@@ -332,9 +332,6 @@
     <t>ex_o</t>
   </si>
   <si>
-    <t>heat3</t>
-  </si>
-  <si>
     <t>kgCO2/MWh electricity</t>
   </si>
   <si>
@@ -614,12 +611,6 @@
     <t>c2</t>
   </si>
   <si>
-    <t>Qavg</t>
-  </si>
-  <si>
-    <t>Vmax</t>
-  </si>
-  <si>
     <t>maxdeviation_pressure.gas.in</t>
   </si>
   <si>
@@ -675,6 +666,69 @@
   </si>
   <si>
     <t>maxdeviation_pressure.wellstream.in</t>
+  </si>
+  <si>
+    <t>pressure_method</t>
+  </si>
+  <si>
+    <t>weymouth</t>
+  </si>
+  <si>
+    <t>darcy-weissbach</t>
+  </si>
+  <si>
+    <t>w3b</t>
+  </si>
+  <si>
+    <t>w3c</t>
+  </si>
+  <si>
+    <t>3 pipes in parallel</t>
+  </si>
+  <si>
+    <t>from platform down to seabed</t>
+  </si>
+  <si>
+    <t>XXQavg</t>
+  </si>
+  <si>
+    <t>XXVmax</t>
+  </si>
+  <si>
+    <t>boiler</t>
+  </si>
+  <si>
+    <t>heatpump</t>
+  </si>
+  <si>
+    <t>TODO: what is the suitable model for wellstream transport</t>
+  </si>
+  <si>
+    <t>guess</t>
+  </si>
+  <si>
+    <t>num_pipes</t>
+  </si>
+  <si>
+    <t>number of pipes in parallel (up to platform)</t>
+  </si>
+  <si>
+    <t>heat dump</t>
+  </si>
+  <si>
+    <t>heatdump</t>
+  </si>
+  <si>
+    <t>computed pressure drop with Q=50/15 is 6-6.164</t>
+  </si>
+  <si>
+    <t>water_intake</t>
+  </si>
+  <si>
+    <t>el_dump</t>
+  </si>
+  <si>
+    <t>XXXQmax</t>
   </si>
 </sst>
 </file>
@@ -1043,10 +1097,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{052C0DB0-0590-4B7A-AC1E-E28475B8C302}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1081,7 +1135,7 @@
         <v>2</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -1100,7 +1154,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F3">
         <v>-1</v>
@@ -1114,7 +1168,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F4">
         <v>2</v>
@@ -1128,7 +1182,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F5">
         <v>2</v>
@@ -1145,7 +1199,7 @@
         <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -1190,7 +1244,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="F9">
         <v>-1</v>
@@ -1204,16 +1258,16 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C10" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -1221,13 +1275,13 @@
         <v>46</v>
       </c>
       <c r="C11" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D11">
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="F11">
         <v>-1.2</v>
@@ -1241,13 +1295,18 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D12">
         <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>196</v>
+        <v>193</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -1258,10 +1317,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00A70904-C380-433D-9493-9658C938F213}">
-  <dimension ref="A1:H55"/>
+  <dimension ref="A1:I67"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1270,7 +1329,7 @@
     <col min="3" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1302,7 +1361,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -1311,7 +1370,7 @@
         <v>66</v>
       </c>
       <c r="D2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -1328,7 +1387,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H3">
         <v>1E-3</v>
@@ -1344,7 +1403,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
@@ -1370,7 +1429,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H6">
         <v>1E-3</v>
@@ -1386,7 +1445,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
@@ -1395,7 +1454,7 @@
         <v>66</v>
       </c>
       <c r="D8" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -1412,7 +1471,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H9">
         <v>1E-3</v>
@@ -1428,7 +1487,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B11" t="s">
         <v>4</v>
@@ -1454,7 +1513,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H12">
         <v>1E-3</v>
@@ -1470,7 +1529,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B14" t="s">
         <v>4</v>
@@ -1496,7 +1555,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H15">
         <v>1E-3</v>
@@ -1510,9 +1569,9 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B17" t="s">
         <v>4</v>
@@ -1521,7 +1580,7 @@
         <v>66</v>
       </c>
       <c r="D17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -1536,15 +1595,15 @@
         <v>500</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H18">
         <v>1E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G19" t="s">
         <v>6</v>
       </c>
@@ -1552,9 +1611,9 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B20" t="s">
         <v>35</v>
@@ -1563,7 +1622,7 @@
         <v>66</v>
       </c>
       <c r="D20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -1575,9 +1634,9 @@
         <v>500</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B21" t="s">
         <v>35</v>
@@ -1598,18 +1657,18 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B22" t="s">
         <v>76</v>
       </c>
       <c r="C22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E22">
         <v>1</v>
@@ -1624,132 +1683,120 @@
         <v>200</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G23" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H23">
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G24" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H24">
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>190</v>
-      </c>
-      <c r="B25" t="s">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G25" t="s">
+        <v>38</v>
+      </c>
+      <c r="H25">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>189</v>
+      </c>
+      <c r="B26" t="s">
         <v>76</v>
       </c>
-      <c r="C25" t="s">
-        <v>131</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="C26" t="s">
+        <v>130</v>
+      </c>
+      <c r="D26" t="s">
         <v>22</v>
       </c>
-      <c r="E25">
-        <v>1</v>
-      </c>
-      <c r="F25">
-        <v>1</v>
-      </c>
-      <c r="G25" t="s">
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26" t="s">
         <v>37</v>
       </c>
-      <c r="H25">
+      <c r="H26">
         <v>200</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="G26" t="s">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G27" t="s">
+        <v>171</v>
+      </c>
+      <c r="H27">
+        <v>6.1639999999999997</v>
+      </c>
+      <c r="I27" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G28" t="s">
         <v>172</v>
       </c>
-      <c r="H26">
+      <c r="H28">
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="G27" t="s">
-        <v>173</v>
-      </c>
-      <c r="H27">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="G28" t="s">
-        <v>147</v>
-      </c>
-      <c r="H28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>184</v>
-      </c>
-      <c r="B29" t="s">
-        <v>63</v>
-      </c>
-      <c r="C29" t="s">
-        <v>22</v>
-      </c>
-      <c r="D29" t="s">
-        <v>65</v>
-      </c>
-      <c r="E29">
-        <v>1</v>
-      </c>
-      <c r="F29">
-        <v>0.01</v>
-      </c>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G29" t="s">
-        <v>37</v>
+        <v>146</v>
       </c>
       <c r="H29">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G30" t="s">
-        <v>172</v>
+        <v>38</v>
       </c>
       <c r="H30">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="G31" t="s">
-        <v>173</v>
-      </c>
-      <c r="H31">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G31" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="H31" s="2">
+        <v>15</v>
+      </c>
+      <c r="I31" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B32" t="s">
         <v>63</v>
       </c>
       <c r="C32" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" t="s">
         <v>65</v>
       </c>
-      <c r="D32" t="s">
-        <v>46</v>
-      </c>
       <c r="E32">
         <v>1</v>
       </c>
       <c r="F32">
-        <v>5</v>
+        <v>0.01</v>
       </c>
       <c r="G32" t="s">
         <v>37</v>
@@ -1760,94 +1807,94 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G33" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H33">
-        <v>5</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G34" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H34">
-        <v>3</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B35" t="s">
+        <v>63</v>
+      </c>
+      <c r="C35" t="s">
+        <v>65</v>
+      </c>
+      <c r="D35" t="s">
+        <v>46</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35">
         <v>5</v>
-      </c>
-      <c r="C35" t="s">
-        <v>22</v>
-      </c>
-      <c r="D35" t="s">
-        <v>29</v>
-      </c>
-      <c r="E35">
-        <v>1</v>
-      </c>
-      <c r="F35">
-        <v>0.01</v>
       </c>
       <c r="G35" t="s">
         <v>37</v>
       </c>
       <c r="H35">
-        <v>500</v>
+        <v>200</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G36" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H36">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G37" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>185</v>
+      </c>
+      <c r="B38" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" t="s">
+        <v>22</v>
+      </c>
+      <c r="D38" t="s">
+        <v>29</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38">
+        <v>0.01</v>
+      </c>
+      <c r="G38" t="s">
+        <v>37</v>
+      </c>
+      <c r="H38">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G39" t="s">
+        <v>171</v>
+      </c>
+      <c r="H39">
         <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="G38" t="s">
-        <v>38</v>
-      </c>
-      <c r="H38">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>187</v>
-      </c>
-      <c r="B39" t="s">
-        <v>5</v>
-      </c>
-      <c r="C39" t="s">
-        <v>29</v>
-      </c>
-      <c r="D39" t="s">
-        <v>46</v>
-      </c>
-      <c r="E39">
-        <v>1</v>
-      </c>
-      <c r="F39">
-        <v>5</v>
-      </c>
-      <c r="G39" t="s">
-        <v>37</v>
-      </c>
-      <c r="H39">
-        <v>200</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
@@ -1855,49 +1902,49 @@
         <v>172</v>
       </c>
       <c r="H40">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G41" t="s">
-        <v>173</v>
+        <v>38</v>
       </c>
       <c r="H41">
-        <v>6</v>
+        <v>300</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>186</v>
+      </c>
+      <c r="B42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" t="s">
+        <v>29</v>
+      </c>
+      <c r="D42" t="s">
+        <v>46</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="F42">
+        <v>5</v>
+      </c>
       <c r="G42" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H42">
-        <v>300</v>
+        <v>200</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>188</v>
-      </c>
-      <c r="B43" t="s">
-        <v>5</v>
-      </c>
-      <c r="C43" t="s">
-        <v>22</v>
-      </c>
-      <c r="D43" t="s">
-        <v>66</v>
-      </c>
-      <c r="E43">
-        <v>1</v>
-      </c>
-      <c r="F43">
-        <v>0.01</v>
-      </c>
       <c r="G43" t="s">
-        <v>37</v>
+        <v>171</v>
       </c>
       <c r="H43">
-        <v>100</v>
+        <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
@@ -1905,49 +1952,49 @@
         <v>172</v>
       </c>
       <c r="H44">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G45" t="s">
-        <v>173</v>
+        <v>38</v>
       </c>
       <c r="H45">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>187</v>
+      </c>
+      <c r="B46" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46" t="s">
+        <v>22</v>
+      </c>
+      <c r="D46" t="s">
+        <v>66</v>
+      </c>
+      <c r="E46">
+        <v>1</v>
+      </c>
+      <c r="F46">
+        <v>0.01</v>
+      </c>
+      <c r="G46" t="s">
+        <v>37</v>
+      </c>
+      <c r="H46">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G47" t="s">
+        <v>171</v>
+      </c>
+      <c r="H47">
         <v>2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="G46" t="s">
-        <v>38</v>
-      </c>
-      <c r="H46">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>182</v>
-      </c>
-      <c r="B47" t="s">
-        <v>64</v>
-      </c>
-      <c r="C47" t="s">
-        <v>114</v>
-      </c>
-      <c r="D47" t="s">
-        <v>205</v>
-      </c>
-      <c r="E47">
-        <v>1</v>
-      </c>
-      <c r="F47">
-        <v>1</v>
-      </c>
-      <c r="G47" t="s">
-        <v>37</v>
-      </c>
-      <c r="H47">
-        <v>100</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
@@ -1955,71 +2002,71 @@
         <v>172</v>
       </c>
       <c r="H48">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G49" t="s">
-        <v>173</v>
+        <v>38</v>
       </c>
       <c r="H49">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B50" t="s">
         <v>64</v>
       </c>
       <c r="C50" t="s">
-        <v>22</v>
+        <v>227</v>
       </c>
       <c r="D50" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E50">
         <v>1</v>
       </c>
       <c r="F50">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="G50" t="s">
         <v>37</v>
       </c>
       <c r="H50">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G51" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H51">
         <v>0.7</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G52" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H52">
         <v>0.7</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>208</v>
+        <v>182</v>
       </c>
       <c r="B53" t="s">
         <v>64</v>
       </c>
       <c r="C53" t="s">
-        <v>205</v>
+        <v>22</v>
       </c>
       <c r="D53" t="s">
-        <v>145</v>
+        <v>202</v>
       </c>
       <c r="E53">
         <v>1</v>
@@ -2031,23 +2078,179 @@
         <v>37</v>
       </c>
       <c r="H53">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G54" t="s">
+        <v>171</v>
+      </c>
+      <c r="H54">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G55" t="s">
         <v>172</v>
       </c>
-      <c r="H54">
+      <c r="H55">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>205</v>
+      </c>
+      <c r="B56" t="s">
+        <v>64</v>
+      </c>
+      <c r="C56" t="s">
+        <v>202</v>
+      </c>
+      <c r="D56" t="s">
+        <v>144</v>
+      </c>
+      <c r="E56">
+        <v>1</v>
+      </c>
+      <c r="F56">
+        <v>1</v>
+      </c>
+      <c r="G56" t="s">
+        <v>37</v>
+      </c>
+      <c r="H56">
+        <v>250</v>
+      </c>
+      <c r="I56" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G57" t="s">
+        <v>171</v>
+      </c>
+      <c r="H57">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G58" t="s">
+        <v>172</v>
+      </c>
+      <c r="H58">
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="G55" t="s">
-        <v>173</v>
-      </c>
-      <c r="H55">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G59" t="s">
+        <v>146</v>
+      </c>
+      <c r="H59">
+        <v>-100</v>
+      </c>
+      <c r="I59" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>212</v>
+      </c>
+      <c r="B60" t="s">
+        <v>64</v>
+      </c>
+      <c r="C60" t="s">
+        <v>202</v>
+      </c>
+      <c r="D60" t="s">
+        <v>144</v>
+      </c>
+      <c r="E60">
+        <v>1</v>
+      </c>
+      <c r="F60">
+        <v>1</v>
+      </c>
+      <c r="G60" t="s">
+        <v>37</v>
+      </c>
+      <c r="H60">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G61" t="s">
+        <v>171</v>
+      </c>
+      <c r="H61">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G62" t="s">
+        <v>172</v>
+      </c>
+      <c r="H62">
         <v>6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G63" t="s">
+        <v>146</v>
+      </c>
+      <c r="H63">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>213</v>
+      </c>
+      <c r="B64" t="s">
+        <v>64</v>
+      </c>
+      <c r="C64" t="s">
+        <v>202</v>
+      </c>
+      <c r="D64" t="s">
+        <v>144</v>
+      </c>
+      <c r="E64">
+        <v>1</v>
+      </c>
+      <c r="F64">
+        <v>1</v>
+      </c>
+      <c r="G64" t="s">
+        <v>37</v>
+      </c>
+      <c r="H64">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="65" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G65" t="s">
+        <v>171</v>
+      </c>
+      <c r="H65">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G66" t="s">
+        <v>172</v>
+      </c>
+      <c r="H66">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="67" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G67" t="s">
+        <v>146</v>
+      </c>
+      <c r="H67">
+        <v>-100</v>
       </c>
     </row>
   </sheetData>
@@ -2057,10 +2260,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB366907-93DA-4245-BEBF-19818450F8D2}">
-  <dimension ref="A1:H75"/>
+  <dimension ref="A1:H77"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="G62" sqref="G62"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2105,7 +2308,7 @@
         <v>34</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
         <v>66</v>
@@ -2133,7 +2336,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>133</v>
+        <v>218</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -2142,513 +2345,519 @@
         <v>66</v>
       </c>
       <c r="D4" t="s">
+        <v>218</v>
+      </c>
+      <c r="E4" t="s">
+        <v>219</v>
+      </c>
+      <c r="F4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" t="s">
         <v>53</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E5" t="s">
         <v>28</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F5" t="s">
         <v>13</v>
       </c>
-      <c r="G4">
+      <c r="G5">
         <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5">
-        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F6" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="G6">
-        <v>2.35</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G7">
-        <v>0.53</v>
+        <v>2.35</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G8">
-        <v>0.05</v>
+        <v>0.53</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F9" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="G9">
-        <v>0.5</v>
-      </c>
-      <c r="H9" t="s">
-        <v>121</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G10">
-        <v>1</v>
+        <v>0.5</v>
+      </c>
+      <c r="H10" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F11" t="s">
-        <v>116</v>
+        <v>55</v>
       </c>
       <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11" t="s">
-        <v>117</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F12" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F13" t="s">
+        <v>122</v>
+      </c>
+      <c r="G13">
         <v>200</v>
       </c>
-      <c r="H12" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>134</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="H13" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>133</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
         <v>66</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D14" t="s">
         <v>52</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E14" t="s">
         <v>28</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F14" t="s">
         <v>13</v>
       </c>
-      <c r="G13">
+      <c r="G14">
         <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F14" t="s">
-        <v>14</v>
-      </c>
-      <c r="G14">
-        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F15" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="G15">
-        <v>2.3519999999999999</v>
-      </c>
-      <c r="H15" t="s">
-        <v>119</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G16">
-        <v>0.53</v>
+        <v>2.3519999999999999</v>
+      </c>
+      <c r="H16" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F17" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G17">
-        <v>0.05</v>
+        <v>0.53</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F18" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="G18">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G19">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F20" t="s">
-        <v>116</v>
+        <v>55</v>
       </c>
       <c r="G20">
-        <v>0</v>
-      </c>
-      <c r="H20" t="s">
-        <v>117</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F21" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F22" t="s">
+        <v>122</v>
+      </c>
+      <c r="G22">
         <v>200</v>
       </c>
-      <c r="H21" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>135</v>
-      </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="H22" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>134</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
         <v>66</v>
       </c>
-      <c r="D22" t="s">
-        <v>126</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="D23" t="s">
+        <v>125</v>
+      </c>
+      <c r="E23" t="s">
         <v>28</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F23" t="s">
         <v>13</v>
       </c>
-      <c r="G22">
+      <c r="G23">
         <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F23" t="s">
-        <v>14</v>
-      </c>
-      <c r="G23">
-        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F24" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="G24">
-        <v>2.3540000000000001</v>
-      </c>
-      <c r="H24" t="s">
-        <v>119</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G25">
-        <v>0.53</v>
+        <v>2.3540000000000001</v>
+      </c>
+      <c r="H25" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F26" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G26">
-        <v>0.05</v>
+        <v>0.53</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F27" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="G27">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G28">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F29" t="s">
-        <v>116</v>
+        <v>55</v>
       </c>
       <c r="G29">
-        <v>0</v>
-      </c>
-      <c r="H29" t="s">
-        <v>117</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F30" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F31" t="s">
+        <v>122</v>
+      </c>
+      <c r="G31">
         <v>200</v>
       </c>
-      <c r="H30" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>140</v>
-      </c>
-      <c r="B31">
+      <c r="H31" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>139</v>
+      </c>
+      <c r="B32">
         <v>0</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C32" t="s">
         <v>66</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D32" t="s">
         <v>19</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E32" t="s">
         <v>44</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F32" t="s">
         <v>45</v>
       </c>
-      <c r="G31">
+      <c r="G32">
         <f>270/0.1</f>
         <v>2700</v>
       </c>
-      <c r="H31" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>136</v>
-      </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
-      <c r="C32" t="s">
+      <c r="H32" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>135</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33" t="s">
         <v>29</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D33" t="s">
         <v>21</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E33" t="s">
         <v>26</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F33" t="s">
         <v>30</v>
       </c>
-      <c r="G32">
+      <c r="G33">
         <v>0.4</v>
-      </c>
-      <c r="H32" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F33" t="s">
-        <v>101</v>
-      </c>
-      <c r="G33">
-        <v>300</v>
       </c>
       <c r="H33" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F34" s="2" t="s">
+      <c r="F34" t="s">
+        <v>100</v>
+      </c>
+      <c r="G34">
+        <v>300</v>
+      </c>
+      <c r="H34" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F35" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G35">
+        <v>20</v>
+      </c>
+      <c r="H35" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="G34">
-        <v>20</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>144</v>
-      </c>
-      <c r="B35">
-        <v>1</v>
-      </c>
-      <c r="C35" t="s">
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>143</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36" t="s">
         <v>22</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D36" t="s">
         <v>22</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E36" t="s">
         <v>22</v>
       </c>
-      <c r="F35" s="2" t="s">
+      <c r="F36" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="G35" s="2">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F36" s="2" t="s">
-        <v>82</v>
       </c>
       <c r="G36" s="2">
         <v>0.1</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+      <c r="F37" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G37" s="2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>136</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38" t="s">
         <v>137</v>
       </c>
-      <c r="B37">
-        <v>1</v>
-      </c>
-      <c r="C37" t="s">
+      <c r="D38" t="s">
         <v>138</v>
       </c>
-      <c r="D37" t="s">
-        <v>139</v>
-      </c>
-      <c r="E37" t="s">
+      <c r="E38" t="s">
         <v>27</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="F38" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G37">
+      <c r="G38">
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F38" s="3" t="s">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F39" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G38">
+      <c r="G39">
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>92</v>
       </c>
-      <c r="B39">
-        <v>1</v>
-      </c>
-      <c r="C39" t="s">
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40" t="s">
         <v>66</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D40" t="s">
         <v>18</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E40" t="s">
         <v>44</v>
       </c>
-      <c r="F39" s="3" t="s">
+      <c r="F40" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G39">
+      <c r="G40">
         <v>20</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F40" t="s">
-        <v>111</v>
-      </c>
-      <c r="G40" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F41" t="s">
+        <v>110</v>
+      </c>
+      <c r="G41" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F42" t="s">
         <v>45</v>
       </c>
-      <c r="G41">
+      <c r="G42">
         <v>0</v>
       </c>
-      <c r="H41" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+      <c r="H42" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>93</v>
       </c>
-      <c r="B42">
-        <v>1</v>
-      </c>
-      <c r="C42" t="s">
-        <v>138</v>
-      </c>
-      <c r="D42" t="s">
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43" t="s">
+        <v>137</v>
+      </c>
+      <c r="D43" t="s">
         <v>10</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E43" t="s">
         <v>33</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F43" t="s">
         <v>13</v>
       </c>
-      <c r="G42">
+      <c r="G43">
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F43" t="s">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F44" t="s">
         <v>14</v>
       </c>
-      <c r="G43">
+      <c r="G44">
         <v>3</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>95</v>
-      </c>
-      <c r="B44">
-        <v>1</v>
-      </c>
-      <c r="C44" t="s">
-        <v>46</v>
-      </c>
-      <c r="D44" t="s">
-        <v>20</v>
-      </c>
-      <c r="E44" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B45">
         <v>1</v>
@@ -2657,246 +2866,237 @@
         <v>46</v>
       </c>
       <c r="D45" t="s">
-        <v>67</v>
+        <v>20</v>
       </c>
       <c r="E45" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46" t="s">
+        <v>46</v>
+      </c>
+      <c r="D46" t="s">
+        <v>67</v>
+      </c>
+      <c r="E46" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>225</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47" t="s">
+        <v>66</v>
+      </c>
+      <c r="D47" t="s">
+        <v>224</v>
+      </c>
+      <c r="E47" t="s">
+        <v>33</v>
+      </c>
+      <c r="F47" t="s">
+        <v>13</v>
+      </c>
+      <c r="G47">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F48" t="s">
+        <v>14</v>
+      </c>
+      <c r="G48">
         <v>0</v>
       </c>
-      <c r="C46" t="s">
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>56</v>
+      </c>
+      <c r="B49">
+        <v>0</v>
+      </c>
+      <c r="C49" t="s">
         <v>66</v>
       </c>
-      <c r="D46" t="s">
-        <v>10</v>
-      </c>
-      <c r="E46" t="s">
-        <v>33</v>
-      </c>
-      <c r="F46" t="s">
+      <c r="D49" t="s">
+        <v>56</v>
+      </c>
+      <c r="E49" t="s">
+        <v>57</v>
+      </c>
+      <c r="F49" t="s">
         <v>13</v>
       </c>
-      <c r="G46">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F47" t="s">
-        <v>14</v>
-      </c>
-      <c r="G47">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>56</v>
-      </c>
-      <c r="B48">
-        <v>0</v>
-      </c>
-      <c r="C48" t="s">
-        <v>66</v>
-      </c>
-      <c r="D48" t="s">
-        <v>56</v>
-      </c>
-      <c r="E48" t="s">
-        <v>57</v>
-      </c>
-      <c r="F48" t="s">
-        <v>13</v>
-      </c>
-      <c r="G48">
+      <c r="G49">
         <v>4</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F49" t="s">
-        <v>14</v>
-      </c>
-      <c r="G49">
-        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F50" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="G50">
-        <v>0.9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F51" t="s">
+        <v>30</v>
+      </c>
+      <c r="G51">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F52" t="s">
         <v>58</v>
       </c>
-      <c r="G51">
+      <c r="G52">
         <v>2</v>
       </c>
-      <c r="H51" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
+      <c r="H52" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
         <v>59</v>
       </c>
-      <c r="B52">
-        <v>1</v>
-      </c>
-      <c r="C52" t="s">
-        <v>114</v>
-      </c>
-      <c r="D52" t="s">
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53" t="s">
+        <v>113</v>
+      </c>
+      <c r="D53" t="s">
         <v>59</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E53" t="s">
         <v>62</v>
       </c>
-      <c r="F52" t="s">
+      <c r="F53" t="s">
+        <v>147</v>
+      </c>
+      <c r="G53">
+        <v>15</v>
+      </c>
+      <c r="H53" t="s">
         <v>148</v>
-      </c>
-      <c r="G52">
-        <v>15</v>
-      </c>
-      <c r="H52" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F53" t="s">
-        <v>39</v>
-      </c>
-      <c r="G53">
-        <v>6</v>
-      </c>
-      <c r="H53" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F54" t="s">
-        <v>111</v>
-      </c>
-      <c r="G54" t="s">
+        <v>39</v>
+      </c>
+      <c r="G54">
+        <v>6</v>
+      </c>
+      <c r="H54" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F55" t="s">
+        <v>110</v>
+      </c>
+      <c r="G55" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
         <v>60</v>
       </c>
-      <c r="B55">
-        <v>1</v>
-      </c>
-      <c r="C55" t="s">
-        <v>114</v>
-      </c>
-      <c r="D55" t="s">
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="C56" t="s">
+        <v>113</v>
+      </c>
+      <c r="D56" t="s">
         <v>60</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E56" t="s">
         <v>62</v>
       </c>
-      <c r="F55" t="s">
-        <v>148</v>
-      </c>
-      <c r="G55">
+      <c r="F56" t="s">
+        <v>147</v>
+      </c>
+      <c r="G56">
         <v>35</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F56" t="s">
-        <v>39</v>
-      </c>
-      <c r="G56">
-        <v>6</v>
-      </c>
-      <c r="H56" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F57" t="s">
-        <v>111</v>
-      </c>
-      <c r="G57" t="s">
+        <v>39</v>
+      </c>
+      <c r="G57">
+        <v>6</v>
+      </c>
+      <c r="H57" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F58" t="s">
+        <v>110</v>
+      </c>
+      <c r="G58" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
         <v>61</v>
       </c>
-      <c r="B58">
+      <c r="B59">
         <v>0</v>
       </c>
-      <c r="C58" t="s">
-        <v>114</v>
-      </c>
-      <c r="D58" t="s">
+      <c r="C59" t="s">
+        <v>113</v>
+      </c>
+      <c r="D59" t="s">
         <v>61</v>
       </c>
-      <c r="E58" t="s">
+      <c r="E59" t="s">
         <v>62</v>
       </c>
-      <c r="F58" t="s">
+      <c r="F59" t="s">
         <v>39</v>
       </c>
-      <c r="G58">
+      <c r="G59">
         <v>6</v>
       </c>
-      <c r="H58" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F59" t="s">
-        <v>148</v>
-      </c>
-      <c r="G59">
-        <v>20</v>
+      <c r="H59" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F60" t="s">
-        <v>111</v>
-      </c>
-      <c r="G60" t="s">
+        <v>147</v>
+      </c>
+      <c r="G60">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F61" t="s">
+        <v>110</v>
+      </c>
+      <c r="G61" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>143</v>
-      </c>
-      <c r="B61">
-        <v>1</v>
-      </c>
-      <c r="C61" t="s">
-        <v>65</v>
-      </c>
-      <c r="D61" t="s">
-        <v>74</v>
-      </c>
-      <c r="E61" t="s">
-        <v>65</v>
-      </c>
-      <c r="F61" t="s">
-        <v>30</v>
-      </c>
-      <c r="G61">
-        <v>0.8</v>
-      </c>
-      <c r="H61" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.3">
@@ -2907,22 +3107,22 @@
         <v>1</v>
       </c>
       <c r="C62" t="s">
-        <v>131</v>
+        <v>65</v>
       </c>
       <c r="D62" t="s">
-        <v>129</v>
+        <v>74</v>
       </c>
       <c r="E62" t="s">
-        <v>130</v>
-      </c>
-      <c r="F62" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F62" t="s">
         <v>30</v>
       </c>
-      <c r="G62" s="2">
-        <v>3</v>
-      </c>
-      <c r="H62" s="2" t="s">
-        <v>132</v>
+      <c r="G62">
+        <v>0.8</v>
+      </c>
+      <c r="H62" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
@@ -2933,77 +3133,95 @@
         <v>1</v>
       </c>
       <c r="C63" t="s">
-        <v>205</v>
+        <v>130</v>
       </c>
       <c r="D63" t="s">
-        <v>207</v>
+        <v>128</v>
       </c>
       <c r="E63" t="s">
-        <v>205</v>
-      </c>
-      <c r="F63" t="s">
+        <v>129</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G63" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="H63" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>140</v>
+      </c>
+      <c r="B64">
+        <v>1</v>
+      </c>
+      <c r="C64" t="s">
+        <v>202</v>
+      </c>
+      <c r="D64" t="s">
+        <v>204</v>
+      </c>
+      <c r="E64" t="s">
+        <v>202</v>
+      </c>
+      <c r="F64" t="s">
         <v>13</v>
       </c>
-      <c r="G63">
+      <c r="G64">
         <v>1000</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F64" t="s">
-        <v>14</v>
-      </c>
-      <c r="G64">
-        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F65" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="G65">
-        <v>0.8</v>
-      </c>
-      <c r="H65" t="s">
-        <v>106</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F66" t="s">
+        <v>30</v>
+      </c>
+      <c r="G66">
+        <v>0.8</v>
+      </c>
+      <c r="H66" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F67" t="s">
+        <v>126</v>
+      </c>
+      <c r="G67">
+        <v>1</v>
+      </c>
+      <c r="H67" t="s">
         <v>127</v>
       </c>
-      <c r="G66">
-        <v>1</v>
-      </c>
-      <c r="H66" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
-        <v>206</v>
-      </c>
-      <c r="B67">
-        <v>1</v>
-      </c>
-      <c r="C67" t="s">
-        <v>145</v>
-      </c>
-      <c r="D67" t="s">
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>203</v>
+      </c>
+      <c r="B68">
+        <v>1</v>
+      </c>
+      <c r="C68" t="s">
+        <v>144</v>
+      </c>
+      <c r="D68" t="s">
         <v>75</v>
       </c>
-      <c r="E67" t="s">
+      <c r="E68" t="s">
         <v>71</v>
       </c>
-      <c r="F67" t="s">
-        <v>148</v>
-      </c>
-      <c r="G67">
-        <v>1.3</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F68" t="s">
-        <v>150</v>
+        <v>229</v>
       </c>
       <c r="G68">
         <v>1.3</v>
@@ -3011,103 +3229,125 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F69" t="s">
-        <v>209</v>
+        <v>149</v>
       </c>
       <c r="G69">
-        <v>6</v>
-      </c>
-      <c r="H69" t="s">
-        <v>107</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F70" t="s">
-        <v>191</v>
+        <v>206</v>
       </c>
       <c r="G70">
-        <v>1.3</v>
+        <v>6</v>
       </c>
       <c r="H70" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F71" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G71">
-        <v>1.3</v>
+        <v>0.3</v>
       </c>
       <c r="H71" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
+      <c r="F72" t="s">
+        <v>217</v>
+      </c>
+      <c r="G72">
+        <v>0</v>
+      </c>
+      <c r="H72" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
         <v>94</v>
       </c>
-      <c r="B72">
-        <v>1</v>
-      </c>
-      <c r="C72" t="s">
+      <c r="B73">
+        <v>1</v>
+      </c>
+      <c r="C73" t="s">
+        <v>227</v>
+      </c>
+      <c r="D73" t="s">
         <v>114</v>
       </c>
-      <c r="D72" t="s">
-        <v>115</v>
-      </c>
-      <c r="E72" t="s">
+      <c r="E73" t="s">
         <v>89</v>
       </c>
-      <c r="F72" t="s">
+      <c r="F73" t="s">
         <v>39</v>
       </c>
-      <c r="G72">
+      <c r="G73">
         <v>0.7</v>
       </c>
-      <c r="H72" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F73" t="s">
+      <c r="H73" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F74" t="s">
+        <v>147</v>
+      </c>
+      <c r="G74">
+        <v>5</v>
+      </c>
+      <c r="H74" t="s">
         <v>148</v>
       </c>
-      <c r="G73">
-        <v>5</v>
-      </c>
-      <c r="H73" t="s">
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>145</v>
+      </c>
+      <c r="B75">
+        <v>0</v>
+      </c>
+      <c r="C75" t="s">
+        <v>144</v>
+      </c>
+      <c r="D75" t="s">
+        <v>70</v>
+      </c>
+      <c r="E75" t="s">
+        <v>71</v>
+      </c>
+      <c r="F75" t="s">
+        <v>147</v>
+      </c>
+      <c r="G75">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F76" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
-        <v>146</v>
-      </c>
-      <c r="B74">
+      <c r="G76">
         <v>0</v>
       </c>
-      <c r="C74" t="s">
-        <v>145</v>
-      </c>
-      <c r="D74" t="s">
-        <v>70</v>
-      </c>
-      <c r="E74" t="s">
-        <v>71</v>
-      </c>
-      <c r="F74" t="s">
-        <v>148</v>
-      </c>
-      <c r="G74">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F75" t="s">
-        <v>150</v>
-      </c>
-      <c r="G75">
-        <v>0</v>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>228</v>
+      </c>
+      <c r="B77">
+        <v>1</v>
+      </c>
+      <c r="C77" t="s">
+        <v>66</v>
+      </c>
+      <c r="E77" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -3118,17 +3358,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B173308-94D5-4307-9C97-06EC5F416B49}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="56.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3143,7 +3383,7 @@
         <v>91</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -3151,162 +3391,156 @@
         <v>76</v>
       </c>
       <c r="B2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C2">
         <v>2E-3</v>
       </c>
       <c r="D2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C3">
         <v>0.995</v>
       </c>
       <c r="D3" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C4">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="D4" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C5">
         <v>5.63</v>
       </c>
       <c r="D5" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C6">
         <v>1E-3</v>
       </c>
       <c r="D6" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>64</v>
-      </c>
       <c r="B7" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C7">
-        <v>1000</v>
-      </c>
-      <c r="D7" t="s">
-        <v>163</v>
+        <v>1E-3</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>152</v>
-      </c>
-      <c r="C8">
-        <v>1E-3</v>
+        <v>209</v>
+      </c>
+      <c r="C8" t="s">
+        <v>211</v>
       </c>
       <c r="D8" t="s">
-        <v>164</v>
+        <v>220</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C9">
-        <v>900</v>
+        <v>1000</v>
       </c>
       <c r="D9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C10">
-        <v>2.5999999999999999E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="D10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>153</v>
-      </c>
-      <c r="C11">
-        <v>419</v>
-      </c>
-      <c r="D11" t="s">
-        <v>165</v>
+        <v>209</v>
+      </c>
+      <c r="C11" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C12">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>63</v>
       </c>
       <c r="B13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C13">
-        <v>0.84</v>
+        <v>900</v>
       </c>
       <c r="D13" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C14">
-        <v>40</v>
+        <v>2.5999999999999999E-3</v>
       </c>
       <c r="D14" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C15">
-        <v>2.34</v>
+        <v>419</v>
       </c>
       <c r="D15" t="s">
-        <v>204</v>
+        <v>164</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -3314,84 +3548,144 @@
         <v>153</v>
       </c>
       <c r="C16">
-        <v>0.41899999999999998</v>
-      </c>
-      <c r="D16" t="s">
-        <v>165</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>157</v>
-      </c>
-      <c r="C17">
+        <v>209</v>
+      </c>
+      <c r="C17" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>150</v>
+      </c>
+      <c r="C18">
+        <v>0.84</v>
+      </c>
+      <c r="D18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>154</v>
+      </c>
+      <c r="C19">
+        <v>40</v>
+      </c>
+      <c r="D19" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>155</v>
+      </c>
+      <c r="C20">
+        <v>2.34</v>
+      </c>
+      <c r="D20" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>152</v>
+      </c>
+      <c r="C21">
+        <v>0.41899999999999998</v>
+      </c>
+      <c r="D21" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>156</v>
+      </c>
+      <c r="C22">
         <f>273+15</f>
         <v>288</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D22" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>157</v>
+      </c>
+      <c r="C23">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="D23" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>158</v>
+      </c>
+      <c r="C24">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>159</v>
+      </c>
+      <c r="C25">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>160</v>
+      </c>
+      <c r="C26">
+        <v>1.27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>161</v>
+      </c>
+      <c r="C27">
+        <v>500</v>
+      </c>
+      <c r="D27" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
-        <v>158</v>
-      </c>
-      <c r="C18">
-        <v>0.10100000000000001</v>
-      </c>
-      <c r="D18" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
-        <v>159</v>
-      </c>
-      <c r="C19">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
-        <v>160</v>
-      </c>
-      <c r="C20">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
-        <v>161</v>
-      </c>
-      <c r="C21">
-        <v>1.27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
-        <v>162</v>
-      </c>
-      <c r="C22">
-        <v>500</v>
-      </c>
-      <c r="D22" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>209</v>
+      </c>
+      <c r="C28" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>35</v>
       </c>
-      <c r="D24" t="s">
-        <v>170</v>
+      <c r="D30" t="s">
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -3405,7 +3699,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3445,7 +3739,7 @@
         <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -3461,13 +3755,13 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B5">
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -3478,7 +3772,7 @@
         <v>0.04</v>
       </c>
       <c r="C6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -3497,7 +3791,7 @@
         <v>72</v>
       </c>
       <c r="B8">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
       <c r="C8" t="s">
         <v>73</v>
@@ -3549,13 +3843,13 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>123</v>
+      </c>
+      <c r="B13">
+        <v>0.8</v>
+      </c>
+      <c r="C13" t="s">
         <v>124</v>
-      </c>
-      <c r="B13">
-        <v>0.5</v>
-      </c>
-      <c r="C13" t="s">
-        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -9973,21 +10267,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010068757AD89D0841429F5831BBC6267AC1" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3e521892cf07d8fee7d1fab9fe3aaa83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="78e0c6f3-9112-4e2d-9710-8a99a0c0b95c" xmlns:ns4="53f6e7f0-9e34-4545-9b50-e54ccadfb78a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3ffc55c83d6521c05fad87c69f289641" ns3:_="" ns4:_="">
     <xsd:import namespace="78e0c6f3-9112-4e2d-9710-8a99a0c0b95c"/>
@@ -10196,24 +10475,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78762D46-3C96-44E4-BFC9-B88DF736E950}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B20FA7CB-4913-4ED5-B2A6-1FAA15DCEB4D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1016DCAE-9D9F-40DE-A38A-1587953D2A7E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10230,4 +10507,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B20FA7CB-4913-4ED5-B2A6-1FAA15DCEB4D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78762D46-3C96-44E4-BFC9-B88DF736E950}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>